<commit_message>
keep taxonomic group add url
</commit_message>
<xml_diff>
--- a/data-raw/data-out/CAN-SARD_data_dictionary.xlsx
+++ b/data-raw/data-out/CAN-SARD_data_dictionary.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="478">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="482">
   <si>
     <t>Column header</t>
   </si>
@@ -49,18 +49,6 @@
     <t>Binomial name of species</t>
   </si>
   <si>
-    <t>Birds</t>
-  </si>
-  <si>
-    <t>Freshwater Fishes</t>
-  </si>
-  <si>
-    <t>Marine Fishes</t>
-  </si>
-  <si>
-    <t>Marine Mammals</t>
-  </si>
-  <si>
     <t>YYYY</t>
   </si>
   <si>
@@ -85,9 +73,6 @@
     <t>0 (no)/1 (yes)</t>
   </si>
   <si>
-    <t>large_taxonomic_group</t>
-  </si>
-  <si>
     <t>EOO</t>
   </si>
   <si>
@@ -217,18 +202,6 @@
     <t>Common name of species and population</t>
   </si>
   <si>
-    <t>Reduce 12 taxonomic groups to 8 groups by combining Reptiles and Amphibians into Herpetofauna, Lichens, Mosses, and Vascular Plants into Plants, and Arthropods and Molluscs into Invertebrates.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Herpetofauna </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Invertebrates </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Plants </t>
-  </si>
-  <si>
     <t>Date that COSEWIC assessment was completed</t>
   </si>
   <si>
@@ -281,9 +254,6 @@
   </si>
   <si>
     <t>From technical summary in status report. When multiple numbers were given the larger was used, if a range was given the mean was used.</t>
-  </si>
-  <si>
-    <t>Aggregated taxonomic group</t>
   </si>
   <si>
     <t>Y (Yes)/P (Partially)/N (No)</t>
@@ -2263,6 +2233,48 @@
   </si>
   <si>
     <t>rowID</t>
+  </si>
+  <si>
+    <t>taxonomic_group</t>
+  </si>
+  <si>
+    <t>Taxonomic group</t>
+  </si>
+  <si>
+    <t>Amphibians</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Arthropods</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Birds</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Fishes (freshwater)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Fishes (marine)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Lichens</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Mammals (marine)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Mammals (terrestrial)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Molluscs</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Mosses</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Reptiles</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Vascular Plants</t>
   </si>
 </sst>
 </file>
@@ -2544,11 +2556,11 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2962,8 +2974,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2973,7 +2985,9 @@
     <col min="3" max="3" width="52.21875" style="24" customWidth="1"/>
     <col min="4" max="10" width="20.6640625" style="24" customWidth="1"/>
     <col min="11" max="11" width="22.44140625" style="24" customWidth="1"/>
-    <col min="12" max="16384" width="8.88671875" style="24"/>
+    <col min="12" max="14" width="8.88671875" style="24"/>
+    <col min="15" max="15" width="18.5546875" style="24" customWidth="1"/>
+    <col min="16" max="16384" width="8.88671875" style="24"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
@@ -2984,7 +2998,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="D1" s="34" t="s">
         <v>2</v>
@@ -3003,16 +3017,16 @@
     </row>
     <row r="2" spans="1:15">
       <c r="A2" s="1" t="s">
-        <v>477</v>
+        <v>467</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>452</v>
+        <v>442</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>453</v>
+        <v>443</v>
       </c>
       <c r="D2" s="27" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="E2" s="26"/>
       <c r="F2" s="26"/>
@@ -3028,16 +3042,16 @@
     </row>
     <row r="3" spans="1:15" ht="28.8">
       <c r="A3" s="1" t="s">
-        <v>476</v>
+        <v>466</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>454</v>
+        <v>444</v>
       </c>
       <c r="D3" s="25" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="E3" s="25"/>
       <c r="F3" s="25"/>
@@ -3056,10 +3070,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>460</v>
+        <v>450</v>
       </c>
       <c r="D4" s="25" t="s">
         <v>4</v>
@@ -3084,7 +3098,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>461</v>
+        <v>451</v>
       </c>
       <c r="D5" s="25" t="s">
         <v>4</v>
@@ -3103,22 +3117,22 @@
     </row>
     <row r="6" spans="1:15" ht="28.8">
       <c r="A6" s="1" t="s">
-        <v>349</v>
+        <v>339</v>
       </c>
       <c r="B6" s="27" t="s">
-        <v>384</v>
+        <v>374</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>385</v>
+        <v>375</v>
       </c>
       <c r="D6" s="24" t="s">
-        <v>381</v>
+        <v>371</v>
       </c>
       <c r="E6" s="26" t="s">
-        <v>382</v>
+        <v>372</v>
       </c>
       <c r="F6" s="26" t="s">
-        <v>383</v>
+        <v>373</v>
       </c>
       <c r="G6" s="26"/>
       <c r="H6" s="26"/>
@@ -3132,22 +3146,22 @@
     </row>
     <row r="7" spans="1:15">
       <c r="A7" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B7" s="28" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C7" s="29" t="s">
-        <v>332</v>
+        <v>322</v>
       </c>
       <c r="D7" s="25" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E7" s="25" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F7" s="25" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G7" s="25"/>
       <c r="H7" s="25"/>
@@ -3161,13 +3175,13 @@
     </row>
     <row r="8" spans="1:15">
       <c r="A8" s="1" t="s">
-        <v>350</v>
+        <v>340</v>
       </c>
       <c r="B8" s="29" t="s">
-        <v>386</v>
+        <v>376</v>
       </c>
       <c r="C8" s="29" t="s">
-        <v>387</v>
+        <v>377</v>
       </c>
       <c r="D8" s="25"/>
       <c r="E8" s="25"/>
@@ -3184,16 +3198,16 @@
     </row>
     <row r="9" spans="1:15" ht="28.8">
       <c r="A9" s="1" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="B9" s="29" t="s">
-        <v>389</v>
+        <v>379</v>
       </c>
       <c r="C9" s="29" t="s">
-        <v>390</v>
+        <v>380</v>
       </c>
       <c r="D9" s="27" t="s">
-        <v>388</v>
+        <v>378</v>
       </c>
       <c r="E9" s="25"/>
       <c r="F9" s="25"/>
@@ -3209,16 +3223,16 @@
     </row>
     <row r="10" spans="1:15">
       <c r="A10" s="1" t="s">
-        <v>352</v>
+        <v>342</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>391</v>
+        <v>381</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>392</v>
+        <v>382</v>
       </c>
       <c r="D10" s="25" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E10" s="25"/>
       <c r="F10" s="25"/>
@@ -3234,16 +3248,16 @@
     </row>
     <row r="11" spans="1:15" ht="28.8">
       <c r="A11" s="1" t="s">
-        <v>353</v>
+        <v>343</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>393</v>
+        <v>383</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>473</v>
+        <v>463</v>
       </c>
       <c r="D11" s="27" t="s">
-        <v>388</v>
+        <v>378</v>
       </c>
       <c r="E11" s="25"/>
       <c r="F11" s="25"/>
@@ -3259,14 +3273,14 @@
     </row>
     <row r="12" spans="1:15" ht="28.8">
       <c r="A12" s="1" t="s">
-        <v>354</v>
+        <v>344</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>394</v>
+        <v>384</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="25" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E12" s="25"/>
       <c r="F12" s="25"/>
@@ -3278,16 +3292,16 @@
     </row>
     <row r="13" spans="1:15" ht="43.2">
       <c r="A13" s="1" t="s">
-        <v>355</v>
+        <v>345</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>395</v>
+        <v>385</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>396</v>
+        <v>386</v>
       </c>
       <c r="D13" s="25" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E13" s="25"/>
       <c r="F13" s="25"/>
@@ -3303,16 +3317,16 @@
     </row>
     <row r="14" spans="1:15" ht="28.8">
       <c r="A14" s="1" t="s">
-        <v>356</v>
+        <v>346</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>397</v>
+        <v>387</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>398</v>
+        <v>388</v>
       </c>
       <c r="D14" s="25" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E14" s="25"/>
       <c r="F14" s="25"/>
@@ -3326,58 +3340,66 @@
       <c r="N14" s="25"/>
       <c r="O14" s="25"/>
     </row>
-    <row r="15" spans="1:15" ht="57.6">
+    <row r="15" spans="1:15">
       <c r="A15" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B15" s="27" t="s">
-        <v>85</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>63</v>
-      </c>
+        <v>468</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="C15" s="1"/>
       <c r="D15" s="25" t="s">
-        <v>7</v>
+        <v>470</v>
       </c>
       <c r="E15" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="F15" s="27" t="s">
-        <v>64</v>
-      </c>
-      <c r="G15" s="27" t="s">
-        <v>65</v>
+        <v>471</v>
+      </c>
+      <c r="F15" s="25" t="s">
+        <v>472</v>
+      </c>
+      <c r="G15" s="25" t="s">
+        <v>473</v>
       </c>
       <c r="H15" s="25" t="s">
-        <v>9</v>
+        <v>474</v>
       </c>
       <c r="I15" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="J15" s="27" t="s">
-        <v>66</v>
-      </c>
-      <c r="K15" s="25"/>
-      <c r="L15" s="25"/>
-      <c r="M15" s="25"/>
-      <c r="N15" s="25"/>
-      <c r="O15" s="25"/>
+        <v>475</v>
+      </c>
+      <c r="J15" s="25" t="s">
+        <v>476</v>
+      </c>
+      <c r="K15" s="25" t="s">
+        <v>477</v>
+      </c>
+      <c r="L15" s="25" t="s">
+        <v>478</v>
+      </c>
+      <c r="M15" s="25" t="s">
+        <v>479</v>
+      </c>
+      <c r="N15" s="25" t="s">
+        <v>480</v>
+      </c>
+      <c r="O15" s="25" t="s">
+        <v>481</v>
+      </c>
     </row>
     <row r="16" spans="1:15" ht="28.8">
       <c r="A16" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>402</v>
+        <v>392</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="D16" s="25" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E16" s="27" t="s">
-        <v>403</v>
+        <v>393</v>
       </c>
       <c r="F16" s="25"/>
       <c r="G16" s="25"/>
@@ -3391,22 +3413,22 @@
     </row>
     <row r="17" spans="1:17" ht="72">
       <c r="A17" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B17" s="27" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="D17" s="24" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="E17" s="27" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="F17" s="27" t="s">
-        <v>403</v>
+        <v>393</v>
       </c>
       <c r="G17" s="25"/>
       <c r="H17" s="25"/>
@@ -3422,22 +3444,22 @@
     </row>
     <row r="18" spans="1:17" ht="57.6">
       <c r="A18" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="D18" s="24" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="E18" s="27" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="F18" s="27" t="s">
-        <v>403</v>
+        <v>393</v>
       </c>
       <c r="G18" s="25"/>
       <c r="H18" s="25"/>
@@ -3451,22 +3473,22 @@
     </row>
     <row r="19" spans="1:17" ht="86.4">
       <c r="A19" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B19" s="27" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="D19" s="27" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="E19" s="27" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="F19" s="27" t="s">
-        <v>403</v>
+        <v>393</v>
       </c>
       <c r="G19" s="25"/>
       <c r="H19" s="25"/>
@@ -3480,19 +3502,19 @@
     </row>
     <row r="20" spans="1:17" ht="28.8">
       <c r="A20" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B20" s="25" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="D20" s="25" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E20" s="27" t="s">
-        <v>403</v>
+        <v>393</v>
       </c>
       <c r="F20" s="27"/>
       <c r="G20" s="25"/>
@@ -3507,19 +3529,19 @@
     </row>
     <row r="21" spans="1:17" ht="28.8">
       <c r="A21" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B21" s="25" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="D21" s="25" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E21" s="27" t="s">
-        <v>403</v>
+        <v>393</v>
       </c>
       <c r="F21" s="27"/>
       <c r="G21" s="25"/>
@@ -3534,19 +3556,19 @@
     </row>
     <row r="22" spans="1:17" ht="57.6">
       <c r="A22" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B22" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>82</v>
-      </c>
       <c r="D22" s="25" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E22" s="27" t="s">
-        <v>403</v>
+        <v>393</v>
       </c>
       <c r="F22" s="27"/>
       <c r="G22" s="25"/>
@@ -3561,31 +3583,31 @@
     </row>
     <row r="23" spans="1:17">
       <c r="A23" s="1" t="s">
-        <v>357</v>
+        <v>347</v>
       </c>
       <c r="B23" s="29" t="s">
-        <v>404</v>
+        <v>394</v>
       </c>
       <c r="C23" s="29" t="s">
-        <v>331</v>
+        <v>321</v>
       </c>
       <c r="D23" s="25" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E23" s="25" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F23" s="25" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G23" s="25" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="H23" s="27" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="I23" s="25" t="s">
-        <v>405</v>
+        <v>395</v>
       </c>
       <c r="J23" s="25"/>
       <c r="K23" s="25"/>
@@ -3595,16 +3617,16 @@
     </row>
     <row r="24" spans="1:17" ht="72">
       <c r="A24" s="1" t="s">
-        <v>358</v>
+        <v>348</v>
       </c>
       <c r="B24" s="24" t="s">
-        <v>400</v>
+        <v>390</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>401</v>
+        <v>391</v>
       </c>
       <c r="D24" s="24" t="s">
-        <v>399</v>
+        <v>389</v>
       </c>
       <c r="I24" s="25"/>
       <c r="K24" s="25"/>
@@ -3615,19 +3637,19 @@
     </row>
     <row r="25" spans="1:17" ht="57.6">
       <c r="A25" s="1" t="s">
-        <v>359</v>
+        <v>349</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>335</v>
+        <v>325</v>
       </c>
       <c r="D25" s="27" t="s">
-        <v>388</v>
+        <v>378</v>
       </c>
       <c r="E25" s="27" t="s">
-        <v>412</v>
+        <v>402</v>
       </c>
       <c r="F25" s="25"/>
       <c r="G25" s="25"/>
@@ -3642,19 +3664,19 @@
     </row>
     <row r="26" spans="1:17" ht="57.6">
       <c r="A26" s="1" t="s">
-        <v>360</v>
+        <v>350</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>333</v>
+        <v>323</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>335</v>
+        <v>325</v>
       </c>
       <c r="D26" s="27" t="s">
-        <v>388</v>
+        <v>378</v>
       </c>
       <c r="E26" s="27" t="s">
-        <v>412</v>
+        <v>402</v>
       </c>
       <c r="F26" s="25"/>
       <c r="G26" s="25"/>
@@ -3669,19 +3691,19 @@
     </row>
     <row r="27" spans="1:17" ht="57.6">
       <c r="A27" s="1" t="s">
-        <v>361</v>
+        <v>351</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>335</v>
+        <v>325</v>
       </c>
       <c r="D27" s="27" t="s">
-        <v>388</v>
+        <v>378</v>
       </c>
       <c r="E27" s="27" t="s">
-        <v>412</v>
+        <v>402</v>
       </c>
       <c r="F27" s="25"/>
       <c r="G27" s="25"/>
@@ -3696,19 +3718,19 @@
     </row>
     <row r="28" spans="1:17" ht="57.6">
       <c r="A28" s="1" t="s">
-        <v>362</v>
+        <v>352</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>335</v>
+        <v>325</v>
       </c>
       <c r="D28" s="27" t="s">
-        <v>388</v>
+        <v>378</v>
       </c>
       <c r="E28" s="27" t="s">
-        <v>412</v>
+        <v>402</v>
       </c>
       <c r="F28" s="25"/>
       <c r="G28" s="25"/>
@@ -3723,19 +3745,19 @@
     </row>
     <row r="29" spans="1:17" ht="57.6">
       <c r="A29" s="1" t="s">
-        <v>363</v>
+        <v>353</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>335</v>
+        <v>325</v>
       </c>
       <c r="D29" s="27" t="s">
-        <v>388</v>
+        <v>378</v>
       </c>
       <c r="E29" s="27" t="s">
-        <v>412</v>
+        <v>402</v>
       </c>
       <c r="F29" s="25"/>
       <c r="G29" s="25"/>
@@ -3750,19 +3772,19 @@
     </row>
     <row r="30" spans="1:17" ht="57.6">
       <c r="A30" s="1" t="s">
-        <v>364</v>
+        <v>354</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>334</v>
+        <v>324</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>335</v>
+        <v>325</v>
       </c>
       <c r="D30" s="27" t="s">
-        <v>388</v>
+        <v>378</v>
       </c>
       <c r="E30" s="27" t="s">
-        <v>412</v>
+        <v>402</v>
       </c>
       <c r="F30" s="25"/>
       <c r="G30" s="25"/>
@@ -3777,28 +3799,28 @@
     </row>
     <row r="31" spans="1:17" ht="57.6">
       <c r="A31" s="1" t="s">
-        <v>365</v>
+        <v>355</v>
       </c>
       <c r="B31" s="27" t="s">
-        <v>411</v>
+        <v>401</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>335</v>
+        <v>325</v>
       </c>
       <c r="D31" s="25" t="s">
-        <v>407</v>
+        <v>397</v>
       </c>
       <c r="E31" s="25" t="s">
-        <v>408</v>
+        <v>398</v>
       </c>
       <c r="F31" s="25" t="s">
-        <v>409</v>
+        <v>399</v>
       </c>
       <c r="G31" s="25" t="s">
-        <v>410</v>
+        <v>400</v>
       </c>
       <c r="H31" s="27" t="s">
-        <v>475</v>
+        <v>465</v>
       </c>
       <c r="I31" s="25"/>
       <c r="J31" s="25"/>
@@ -3809,19 +3831,19 @@
     </row>
     <row r="32" spans="1:17" ht="100.8">
       <c r="A32" s="1" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="C32" s="29" t="s">
-        <v>417</v>
+        <v>407</v>
       </c>
       <c r="D32" s="26" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="E32" s="27" t="s">
-        <v>416</v>
+        <v>406</v>
       </c>
       <c r="F32" s="26"/>
       <c r="G32" s="26"/>
@@ -3836,19 +3858,19 @@
     </row>
     <row r="33" spans="1:15" ht="57.6">
       <c r="A33" s="1" t="s">
-        <v>337</v>
+        <v>327</v>
       </c>
       <c r="B33" s="24" t="s">
-        <v>339</v>
+        <v>329</v>
       </c>
       <c r="C33" s="24" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="D33" s="24" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="E33" s="27" t="s">
-        <v>414</v>
+        <v>404</v>
       </c>
       <c r="L33" s="26"/>
       <c r="M33" s="26"/>
@@ -3857,13 +3879,13 @@
     </row>
     <row r="34" spans="1:15" ht="57.6">
       <c r="A34" s="1" t="s">
-        <v>366</v>
+        <v>356</v>
       </c>
       <c r="B34" s="24" t="s">
-        <v>413</v>
+        <v>403</v>
       </c>
       <c r="D34" s="27" t="s">
-        <v>414</v>
+        <v>404</v>
       </c>
       <c r="L34" s="26"/>
       <c r="M34" s="26"/>
@@ -3872,19 +3894,19 @@
     </row>
     <row r="35" spans="1:15" ht="57.6">
       <c r="A35" s="1" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="B35" s="24" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="C35" s="24" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="D35" s="25" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E35" s="27" t="s">
-        <v>414</v>
+        <v>404</v>
       </c>
       <c r="L35" s="26"/>
       <c r="M35" s="26"/>
@@ -3893,19 +3915,19 @@
     </row>
     <row r="36" spans="1:15" ht="43.2">
       <c r="A36" s="1" t="s">
-        <v>338</v>
+        <v>328</v>
       </c>
       <c r="B36" s="24" t="s">
-        <v>341</v>
+        <v>331</v>
       </c>
       <c r="C36" s="29" t="s">
-        <v>343</v>
+        <v>333</v>
       </c>
       <c r="D36" s="24" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="E36" s="24" t="s">
-        <v>415</v>
+        <v>405</v>
       </c>
       <c r="L36" s="26"/>
       <c r="M36" s="26"/>
@@ -3914,13 +3936,13 @@
     </row>
     <row r="37" spans="1:15" ht="57.6">
       <c r="A37" s="1" t="s">
-        <v>367</v>
+        <v>357</v>
       </c>
       <c r="B37" s="24" t="s">
-        <v>413</v>
+        <v>403</v>
       </c>
       <c r="D37" s="27" t="s">
-        <v>414</v>
+        <v>404</v>
       </c>
       <c r="L37" s="26"/>
       <c r="M37" s="26"/>
@@ -3929,19 +3951,19 @@
     </row>
     <row r="38" spans="1:15" ht="28.8">
       <c r="A38" s="1" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="B38" s="24" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="C38" s="24" t="s">
-        <v>340</v>
+        <v>330</v>
       </c>
       <c r="D38" s="24" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="E38" s="27" t="s">
-        <v>414</v>
+        <v>404</v>
       </c>
       <c r="F38" s="25"/>
       <c r="G38" s="25"/>
@@ -3956,19 +3978,19 @@
     </row>
     <row r="39" spans="1:15" ht="43.2">
       <c r="A39" s="1" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="B39" s="24" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="C39" s="29" t="s">
-        <v>342</v>
+        <v>332</v>
       </c>
       <c r="D39" s="24" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="E39" s="24" t="s">
-        <v>415</v>
+        <v>405</v>
       </c>
       <c r="F39" s="25"/>
       <c r="G39" s="25"/>
@@ -3983,16 +4005,16 @@
     </row>
     <row r="40" spans="1:15" ht="43.2">
       <c r="A40" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B40" s="27" t="s">
-        <v>419</v>
+        <v>409</v>
       </c>
       <c r="C40" s="27" t="s">
-        <v>420</v>
+        <v>410</v>
       </c>
       <c r="D40" s="25" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E40" s="25"/>
       <c r="F40" s="25"/>
@@ -4008,16 +4030,16 @@
     </row>
     <row r="41" spans="1:15" ht="72.599999999999994" thickBot="1">
       <c r="A41" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B41" s="27" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="C41" s="27" t="s">
-        <v>455</v>
+        <v>445</v>
       </c>
       <c r="D41" s="25" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E41" s="25"/>
       <c r="F41" s="25"/>
@@ -4033,13 +4055,13 @@
     </row>
     <row r="42" spans="1:15" ht="58.2" thickBot="1">
       <c r="A42" s="1" t="s">
-        <v>368</v>
+        <v>358</v>
       </c>
       <c r="B42" s="30" t="s">
-        <v>435</v>
+        <v>425</v>
       </c>
       <c r="C42" s="27" t="s">
-        <v>437</v>
+        <v>427</v>
       </c>
       <c r="D42" s="27">
         <v>0</v>
@@ -4048,10 +4070,10 @@
         <v>1</v>
       </c>
       <c r="F42" s="27" t="s">
-        <v>406</v>
+        <v>396</v>
       </c>
       <c r="G42" s="27" t="s">
-        <v>436</v>
+        <v>426</v>
       </c>
       <c r="H42" s="25"/>
       <c r="I42" s="25"/>
@@ -4063,13 +4085,13 @@
     </row>
     <row r="43" spans="1:15" ht="101.4" thickBot="1">
       <c r="A43" s="1" t="s">
-        <v>369</v>
+        <v>359</v>
       </c>
       <c r="B43" s="31" t="s">
-        <v>438</v>
+        <v>428</v>
       </c>
       <c r="C43" s="27" t="s">
-        <v>457</v>
+        <v>447</v>
       </c>
       <c r="D43" s="27">
         <v>0</v>
@@ -4078,10 +4100,10 @@
         <v>1</v>
       </c>
       <c r="F43" s="27" t="s">
-        <v>406</v>
+        <v>396</v>
       </c>
       <c r="G43" s="27" t="s">
-        <v>436</v>
+        <v>426</v>
       </c>
       <c r="H43" s="26"/>
       <c r="I43" s="25"/>
@@ -4093,13 +4115,13 @@
     </row>
     <row r="44" spans="1:15" ht="101.4" thickBot="1">
       <c r="A44" s="1" t="s">
-        <v>370</v>
+        <v>360</v>
       </c>
       <c r="B44" s="31" t="s">
-        <v>439</v>
+        <v>429</v>
       </c>
       <c r="C44" s="27" t="s">
-        <v>457</v>
+        <v>447</v>
       </c>
       <c r="D44" s="27">
         <v>0</v>
@@ -4108,10 +4130,10 @@
         <v>1</v>
       </c>
       <c r="F44" s="27" t="s">
-        <v>406</v>
+        <v>396</v>
       </c>
       <c r="G44" s="27" t="s">
-        <v>436</v>
+        <v>426</v>
       </c>
       <c r="H44" s="26"/>
       <c r="I44" s="26"/>
@@ -4123,13 +4145,13 @@
     </row>
     <row r="45" spans="1:15" ht="101.4" thickBot="1">
       <c r="A45" s="1" t="s">
-        <v>371</v>
+        <v>361</v>
       </c>
       <c r="B45" s="31" t="s">
-        <v>440</v>
+        <v>430</v>
       </c>
       <c r="C45" s="27" t="s">
-        <v>457</v>
+        <v>447</v>
       </c>
       <c r="D45" s="27">
         <v>0</v>
@@ -4138,21 +4160,21 @@
         <v>1</v>
       </c>
       <c r="F45" s="27" t="s">
-        <v>406</v>
+        <v>396</v>
       </c>
       <c r="G45" s="27" t="s">
-        <v>436</v>
+        <v>426</v>
       </c>
     </row>
     <row r="46" spans="1:15" ht="101.4" thickBot="1">
       <c r="A46" s="1" t="s">
-        <v>372</v>
+        <v>362</v>
       </c>
       <c r="B46" s="31" t="s">
-        <v>441</v>
+        <v>431</v>
       </c>
       <c r="C46" s="27" t="s">
-        <v>457</v>
+        <v>447</v>
       </c>
       <c r="D46" s="27">
         <v>0</v>
@@ -4161,67 +4183,67 @@
         <v>1</v>
       </c>
       <c r="F46" s="27" t="s">
-        <v>406</v>
+        <v>396</v>
       </c>
       <c r="G46" s="27" t="s">
-        <v>436</v>
+        <v>426</v>
       </c>
     </row>
     <row r="47" spans="1:15" ht="187.2">
       <c r="A47" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B47" s="27" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="C47" s="27" t="s">
-        <v>458</v>
+        <v>448</v>
       </c>
       <c r="D47" s="25" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E47" s="25"/>
       <c r="F47" s="25"/>
     </row>
     <row r="48" spans="1:15" ht="100.8">
       <c r="A48" s="1" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="B48" s="24" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="C48" s="29" t="s">
-        <v>459</v>
+        <v>449</v>
       </c>
       <c r="D48" s="26" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="E48" s="27"/>
       <c r="F48" s="26"/>
     </row>
     <row r="49" spans="1:16" ht="28.8">
       <c r="A49" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B49" s="27" t="s">
-        <v>418</v>
+        <v>408</v>
       </c>
       <c r="D49" s="25" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E49" s="25" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
     </row>
     <row r="50" spans="1:16" ht="72">
       <c r="A50" s="1" t="s">
-        <v>373</v>
+        <v>363</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>421</v>
+        <v>411</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>456</v>
+        <v>446</v>
       </c>
       <c r="D50" s="1">
         <v>1.1000000000000001</v>
@@ -4230,7 +4252,7 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>433</v>
+        <v>423</v>
       </c>
       <c r="G50" s="1"/>
       <c r="H50" s="1"/>
@@ -4244,19 +4266,19 @@
     </row>
     <row r="51" spans="1:16" ht="28.8">
       <c r="A51" s="1" t="s">
-        <v>374</v>
+        <v>364</v>
       </c>
       <c r="B51" s="24" t="s">
-        <v>422</v>
+        <v>412</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>468</v>
+        <v>458</v>
       </c>
       <c r="D51" s="24" t="s">
-        <v>388</v>
+        <v>378</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>434</v>
+        <v>424</v>
       </c>
       <c r="G51" s="1"/>
       <c r="I51" s="1"/>
@@ -4270,19 +4292,19 @@
     </row>
     <row r="52" spans="1:16" ht="28.8">
       <c r="A52" s="1" t="s">
-        <v>375</v>
+        <v>365</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>423</v>
+        <v>413</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>468</v>
+        <v>458</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>434</v>
+        <v>424</v>
       </c>
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
@@ -4297,19 +4319,19 @@
     </row>
     <row r="53" spans="1:16" ht="28.8">
       <c r="A53" s="1" t="s">
-        <v>376</v>
+        <v>366</v>
       </c>
       <c r="B53" s="24" t="s">
-        <v>424</v>
+        <v>414</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>468</v>
+        <v>458</v>
       </c>
       <c r="D53" s="24" t="s">
         <v>4</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>434</v>
+        <v>424</v>
       </c>
       <c r="G53" s="1"/>
       <c r="I53" s="1"/>
@@ -4322,31 +4344,31 @@
     </row>
     <row r="54" spans="1:16" ht="28.8">
       <c r="A54" s="1" t="s">
-        <v>377</v>
+        <v>367</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>425</v>
+        <v>415</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>470</v>
+        <v>460</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>426</v>
+        <v>416</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>427</v>
+        <v>417</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>428</v>
+        <v>418</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>429</v>
+        <v>419</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>434</v>
+        <v>424</v>
       </c>
       <c r="J54" s="26"/>
       <c r="K54" s="26"/>
@@ -4357,31 +4379,31 @@
     </row>
     <row r="55" spans="1:16" ht="28.8">
       <c r="A55" s="1" t="s">
-        <v>378</v>
+        <v>368</v>
       </c>
       <c r="B55" s="24" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>469</v>
+        <v>459</v>
       </c>
       <c r="D55" s="24" t="s">
         <v>4</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>426</v>
+        <v>416</v>
       </c>
       <c r="F55" s="24" t="s">
-        <v>427</v>
+        <v>417</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>428</v>
+        <v>418</v>
       </c>
       <c r="H55" s="24" t="s">
-        <v>429</v>
+        <v>419</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>434</v>
+        <v>424</v>
       </c>
       <c r="J55" s="26"/>
       <c r="K55" s="26"/>
@@ -4392,19 +4414,19 @@
     </row>
     <row r="56" spans="1:16" ht="28.8">
       <c r="A56" s="1" t="s">
-        <v>379</v>
+        <v>369</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>431</v>
+        <v>421</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>468</v>
+        <v>458</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>434</v>
+        <v>424</v>
       </c>
       <c r="F56" s="1"/>
       <c r="G56" s="1"/>
@@ -4419,19 +4441,19 @@
     </row>
     <row r="57" spans="1:16" ht="28.8">
       <c r="A57" s="1" t="s">
-        <v>380</v>
+        <v>370</v>
       </c>
       <c r="B57" s="24" t="s">
-        <v>432</v>
+        <v>422</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>468</v>
+        <v>458</v>
       </c>
       <c r="D57" s="24" t="s">
         <v>4</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>434</v>
+        <v>424</v>
       </c>
       <c r="G57" s="1"/>
       <c r="I57" s="1"/>
@@ -4444,16 +4466,16 @@
     </row>
     <row r="58" spans="1:16" ht="158.4">
       <c r="A58" s="1" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>449</v>
+        <v>439</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>450</v>
+        <v>440</v>
       </c>
       <c r="D58" s="24" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E58" s="25"/>
       <c r="F58" s="25"/>
@@ -4469,13 +4491,13 @@
     </row>
     <row r="59" spans="1:16" ht="158.4">
       <c r="A59" s="1" t="s">
-        <v>447</v>
+        <v>437</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>448</v>
+        <v>438</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>451</v>
+        <v>441</v>
       </c>
       <c r="D59" s="24">
         <v>0</v>
@@ -4498,169 +4520,169 @@
     </row>
     <row r="60" spans="1:16" ht="72">
       <c r="A60" s="1" t="s">
-        <v>327</v>
+        <v>317</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>462</v>
+        <v>452</v>
       </c>
       <c r="D60" s="27" t="s">
-        <v>442</v>
+        <v>432</v>
       </c>
       <c r="E60" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G60" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="H60" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I60" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J60" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F60" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="G60" s="25" t="s">
-        <v>38</v>
-      </c>
-      <c r="H60" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="I60" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="J60" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="K60" s="32" t="s">
-        <v>444</v>
+        <v>434</v>
       </c>
       <c r="L60" s="33" t="s">
-        <v>445</v>
+        <v>435</v>
       </c>
       <c r="M60" s="1" t="s">
-        <v>446</v>
+        <v>436</v>
       </c>
       <c r="N60" s="25"/>
       <c r="O60" s="25"/>
     </row>
     <row r="61" spans="1:16" ht="72">
       <c r="A61" s="1" t="s">
-        <v>328</v>
+        <v>318</v>
       </c>
       <c r="B61" s="24" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>463</v>
+        <v>453</v>
       </c>
       <c r="D61" s="27" t="s">
-        <v>442</v>
+        <v>432</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="I61" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="J61" s="1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="K61" s="32" t="s">
-        <v>444</v>
+        <v>434</v>
       </c>
       <c r="L61" s="33" t="s">
-        <v>445</v>
+        <v>435</v>
       </c>
       <c r="M61" s="1" t="s">
-        <v>446</v>
+        <v>436</v>
       </c>
       <c r="N61" s="25"/>
       <c r="O61" s="25"/>
     </row>
     <row r="62" spans="1:16" ht="115.2">
       <c r="A62" s="1" t="s">
-        <v>329</v>
+        <v>319</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>464</v>
+        <v>454</v>
       </c>
       <c r="D62" s="27" t="s">
-        <v>442</v>
+        <v>432</v>
       </c>
       <c r="E62" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G62" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H62" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I62" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="J62" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="F62" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="G62" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="H62" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="I62" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="J62" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="K62" s="32" t="s">
-        <v>444</v>
+        <v>434</v>
       </c>
       <c r="L62" s="33" t="s">
-        <v>445</v>
+        <v>435</v>
       </c>
       <c r="M62" s="1" t="s">
-        <v>446</v>
+        <v>436</v>
       </c>
       <c r="N62" s="25"/>
       <c r="O62" s="25"/>
     </row>
     <row r="63" spans="1:16" ht="72">
       <c r="A63" s="1" t="s">
-        <v>330</v>
+        <v>320</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>465</v>
+        <v>455</v>
       </c>
       <c r="D63" s="27" t="s">
-        <v>443</v>
+        <v>433</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="H63" s="1" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="I63" s="1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="J63" s="32" t="s">
-        <v>444</v>
+        <v>434</v>
       </c>
       <c r="K63" s="33" t="s">
-        <v>445</v>
+        <v>435</v>
       </c>
       <c r="L63" s="1" t="s">
-        <v>446</v>
+        <v>436</v>
       </c>
       <c r="M63" s="25"/>
       <c r="N63" s="25"/>
@@ -4668,36 +4690,36 @@
     </row>
     <row r="64" spans="1:16" ht="28.8">
       <c r="A64" s="1" t="s">
-        <v>466</v>
+        <v>456</v>
       </c>
       <c r="B64" s="24" t="s">
-        <v>467</v>
+        <v>457</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>468</v>
+        <v>458</v>
       </c>
       <c r="D64" s="24" t="s">
         <v>4</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>434</v>
+        <v>424</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="43.2">
       <c r="A65" s="1" t="s">
-        <v>471</v>
+        <v>461</v>
       </c>
       <c r="B65" s="24" t="s">
-        <v>474</v>
+        <v>464</v>
       </c>
       <c r="C65" s="24" t="s">
-        <v>472</v>
+        <v>462</v>
       </c>
       <c r="D65" s="24" t="s">
         <v>4</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>434</v>
+        <v>424</v>
       </c>
     </row>
   </sheetData>
@@ -4709,7 +4731,7 @@
       <formula>C22&lt;&gt;#REF!</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B47 B16:C16 B18:C18 B3:C3 B25:C30 B62:C63 C48 B58:C60 B10:C14 C15 C17:C21 C23:C24 C26:C31 C61:C63 C4:C10 C2">
+  <conditionalFormatting sqref="B47 B18:C18 B3:C3 B25:C30 B62:C63 C48 B58:C60 B10:C16 C17:C21 C23:C24 C26:C31 C61:C63 C4:C10 C2">
     <cfRule type="expression" dxfId="14" priority="23">
       <formula>B2&lt;&gt;#REF!</formula>
     </cfRule>
@@ -4806,10 +4828,10 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="4" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>1</v>
@@ -4817,178 +4839,178 @@
     </row>
     <row r="2" spans="1:3" ht="43.2">
       <c r="A2" s="3" t="s">
-        <v>336</v>
+        <v>326</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>345</v>
+        <v>335</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="28.8">
       <c r="A3" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>336</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>346</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="57.6" customHeight="1">
       <c r="A4" s="3" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>347</v>
+        <v>337</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="58.2" customHeight="1">
       <c r="A5" s="3" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>348</v>
+        <v>338</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="43.2">
       <c r="A6" s="3" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="43.2">
       <c r="A7" s="3" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="28.8">
       <c r="A8" s="3" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="57.6">
       <c r="A9" s="3" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="14.4" customHeight="1">
       <c r="A10" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>96</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="28.8">
       <c r="A11" s="3" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>344</v>
+        <v>334</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="28.8">
       <c r="A12" s="3" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="28.8">
       <c r="A13" s="3" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="43.2">
       <c r="A14" s="3" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="28.8">
       <c r="A15" s="3" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="28.8">
       <c r="A16" s="3" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>118</v>
-      </c>
       <c r="C17" s="3" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -5018,7 +5040,7 @@
   <sheetData>
     <row r="1" spans="1:25" ht="14.25" customHeight="1">
       <c r="A1" s="5" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -5047,12 +5069,12 @@
     </row>
     <row r="2" spans="1:25" ht="14.25" customHeight="1">
       <c r="A2" s="8" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
       <c r="D2" s="10" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="E2" s="9"/>
       <c r="F2" s="6"/>
@@ -5078,7 +5100,7 @@
     </row>
     <row r="3" spans="1:25" ht="14.25" customHeight="1">
       <c r="A3" s="11" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="B3" s="12"/>
       <c r="C3" s="12"/>
@@ -5113,13 +5135,13 @@
         <v>2</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="E4" s="16" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
@@ -5143,16 +5165,16 @@
       <c r="Y4" s="6"/>
     </row>
     <row r="5" spans="1:25" ht="14.25" customHeight="1">
-      <c r="A5" s="40" t="s">
-        <v>142</v>
-      </c>
-      <c r="B5" s="41"/>
-      <c r="C5" s="41"/>
+      <c r="A5" s="39" t="s">
+        <v>132</v>
+      </c>
+      <c r="B5" s="40"/>
+      <c r="C5" s="40"/>
       <c r="D5" s="13" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
@@ -5178,14 +5200,14 @@
     <row r="6" spans="1:25" ht="14.25" customHeight="1">
       <c r="A6" s="18"/>
       <c r="B6" s="36" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="C6" s="37"/>
       <c r="D6" s="38" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="E6" s="38" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
@@ -5212,7 +5234,7 @@
       <c r="A7" s="18"/>
       <c r="B7" s="19"/>
       <c r="C7" s="19" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="D7" s="37"/>
       <c r="E7" s="37"/>
@@ -5240,14 +5262,14 @@
     <row r="8" spans="1:25" ht="14.25" customHeight="1">
       <c r="A8" s="18"/>
       <c r="B8" s="36" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="C8" s="37"/>
       <c r="D8" s="38" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="E8" s="38" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
@@ -5274,7 +5296,7 @@
       <c r="A9" s="18"/>
       <c r="B9" s="19"/>
       <c r="C9" s="19" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="D9" s="37"/>
       <c r="E9" s="37"/>
@@ -5302,14 +5324,14 @@
     <row r="10" spans="1:25" ht="14.25" customHeight="1">
       <c r="A10" s="18"/>
       <c r="B10" s="36" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="C10" s="37"/>
       <c r="D10" s="38" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="E10" s="38" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
@@ -5336,7 +5358,7 @@
       <c r="A11" s="18"/>
       <c r="B11" s="19"/>
       <c r="C11" s="19" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="D11" s="37"/>
       <c r="E11" s="37"/>
@@ -5362,16 +5384,16 @@
       <c r="Y11" s="6"/>
     </row>
     <row r="12" spans="1:25" ht="14.25" customHeight="1">
-      <c r="A12" s="40" t="s">
-        <v>157</v>
-      </c>
-      <c r="B12" s="41"/>
-      <c r="C12" s="41"/>
+      <c r="A12" s="39" t="s">
+        <v>147</v>
+      </c>
+      <c r="B12" s="40"/>
+      <c r="C12" s="40"/>
       <c r="D12" s="13" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="E12" s="13" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
@@ -5397,11 +5419,11 @@
     <row r="13" spans="1:25" ht="14.25" customHeight="1">
       <c r="A13" s="18"/>
       <c r="B13" s="36" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="C13" s="37"/>
       <c r="D13" s="38" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="E13" s="38"/>
       <c r="F13" s="6"/>
@@ -5429,7 +5451,7 @@
       <c r="A14" s="18"/>
       <c r="B14" s="18"/>
       <c r="C14" s="19" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="D14" s="37"/>
       <c r="E14" s="37"/>
@@ -5457,14 +5479,14 @@
     <row r="15" spans="1:25" ht="14.25" customHeight="1">
       <c r="A15" s="18"/>
       <c r="B15" s="36" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="C15" s="37"/>
       <c r="D15" s="38" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="E15" s="38" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
@@ -5491,7 +5513,7 @@
       <c r="A16" s="18"/>
       <c r="B16" s="18"/>
       <c r="C16" s="19" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="D16" s="37"/>
       <c r="E16" s="37"/>
@@ -5519,14 +5541,14 @@
     <row r="17" spans="1:25" ht="14.25" customHeight="1">
       <c r="A17" s="18"/>
       <c r="B17" s="36" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="C17" s="37"/>
       <c r="D17" s="38" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="E17" s="38" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="F17" s="6"/>
       <c r="G17" s="6"/>
@@ -5553,7 +5575,7 @@
       <c r="A18" s="18"/>
       <c r="B18" s="18"/>
       <c r="C18" s="19" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="D18" s="37"/>
       <c r="E18" s="37"/>
@@ -5581,14 +5603,14 @@
     <row r="19" spans="1:25" ht="14.25" customHeight="1">
       <c r="A19" s="18"/>
       <c r="B19" s="36" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="C19" s="37"/>
       <c r="D19" s="38" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="E19" s="38" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
@@ -5615,7 +5637,7 @@
       <c r="A20" s="18"/>
       <c r="B20" s="18"/>
       <c r="C20" s="19" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="D20" s="37"/>
       <c r="E20" s="37"/>
@@ -5641,16 +5663,16 @@
       <c r="Y20" s="6"/>
     </row>
     <row r="21" spans="1:25" ht="14.25" customHeight="1">
-      <c r="A21" s="40" t="s">
-        <v>175</v>
-      </c>
-      <c r="B21" s="41"/>
-      <c r="C21" s="41"/>
+      <c r="A21" s="39" t="s">
+        <v>165</v>
+      </c>
+      <c r="B21" s="40"/>
+      <c r="C21" s="40"/>
       <c r="D21" s="13" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="E21" s="13" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
@@ -5676,14 +5698,14 @@
     <row r="22" spans="1:25" ht="14.25" customHeight="1">
       <c r="A22" s="18"/>
       <c r="B22" s="36" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="C22" s="37"/>
       <c r="D22" s="38" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="E22" s="38" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="F22" s="6"/>
       <c r="G22" s="6"/>
@@ -5710,7 +5732,7 @@
       <c r="A23" s="18"/>
       <c r="B23" s="18"/>
       <c r="C23" s="19" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="D23" s="37"/>
       <c r="E23" s="37"/>
@@ -5738,14 +5760,14 @@
     <row r="24" spans="1:25" ht="14.25" customHeight="1">
       <c r="A24" s="18"/>
       <c r="B24" s="36" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="C24" s="37"/>
       <c r="D24" s="38" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="E24" s="38" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="F24" s="6"/>
       <c r="G24" s="6"/>
@@ -5772,7 +5794,7 @@
       <c r="A25" s="18"/>
       <c r="B25" s="18"/>
       <c r="C25" s="19" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
       <c r="D25" s="37"/>
       <c r="E25" s="37"/>
@@ -5800,14 +5822,14 @@
     <row r="26" spans="1:25" ht="14.25" customHeight="1">
       <c r="A26" s="18"/>
       <c r="B26" s="36" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="C26" s="37"/>
       <c r="D26" s="38" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="E26" s="38" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="F26" s="6"/>
       <c r="G26" s="6"/>
@@ -5834,7 +5856,7 @@
       <c r="A27" s="18"/>
       <c r="B27" s="18"/>
       <c r="C27" s="19" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="D27" s="37"/>
       <c r="E27" s="37"/>
@@ -5860,16 +5882,16 @@
       <c r="Y27" s="6"/>
     </row>
     <row r="28" spans="1:25" ht="14.25" customHeight="1">
-      <c r="A28" s="40" t="s">
-        <v>190</v>
-      </c>
-      <c r="B28" s="41"/>
-      <c r="C28" s="41"/>
+      <c r="A28" s="39" t="s">
+        <v>180</v>
+      </c>
+      <c r="B28" s="40"/>
+      <c r="C28" s="40"/>
       <c r="D28" s="13" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="E28" s="13" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="F28" s="6"/>
       <c r="G28" s="6"/>
@@ -5895,14 +5917,14 @@
     <row r="29" spans="1:25" ht="14.25" customHeight="1">
       <c r="A29" s="18"/>
       <c r="B29" s="36" t="s">
-        <v>193</v>
+        <v>183</v>
       </c>
       <c r="C29" s="37"/>
       <c r="D29" s="38" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
       <c r="E29" s="38" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
       <c r="F29" s="6"/>
       <c r="G29" s="6"/>
@@ -5929,7 +5951,7 @@
       <c r="A30" s="18"/>
       <c r="B30" s="18"/>
       <c r="C30" s="19" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="D30" s="37"/>
       <c r="E30" s="37"/>
@@ -5957,14 +5979,14 @@
     <row r="31" spans="1:25" ht="14.25" customHeight="1">
       <c r="A31" s="18"/>
       <c r="B31" s="36" t="s">
-        <v>197</v>
+        <v>187</v>
       </c>
       <c r="C31" s="37"/>
       <c r="D31" s="38" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="E31" s="38" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
       <c r="F31" s="6"/>
       <c r="G31" s="6"/>
@@ -5991,7 +6013,7 @@
       <c r="A32" s="18"/>
       <c r="B32" s="18"/>
       <c r="C32" s="19" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="D32" s="37"/>
       <c r="E32" s="37"/>
@@ -6019,14 +6041,14 @@
     <row r="33" spans="1:25" ht="14.25" customHeight="1">
       <c r="A33" s="18"/>
       <c r="B33" s="36" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
       <c r="C33" s="37"/>
       <c r="D33" s="38" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="E33" s="38" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
       <c r="F33" s="6"/>
       <c r="G33" s="6"/>
@@ -6053,7 +6075,7 @@
       <c r="A34" s="18"/>
       <c r="B34" s="18"/>
       <c r="C34" s="19" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="D34" s="37"/>
       <c r="E34" s="37"/>
@@ -6081,14 +6103,14 @@
     <row r="35" spans="1:25" ht="14.25" customHeight="1">
       <c r="A35" s="18"/>
       <c r="B35" s="36" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="C35" s="37"/>
       <c r="D35" s="38" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
       <c r="E35" s="38" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
       <c r="F35" s="6"/>
       <c r="G35" s="6"/>
@@ -6115,7 +6137,7 @@
       <c r="A36" s="18"/>
       <c r="B36" s="18"/>
       <c r="C36" s="19" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="D36" s="37"/>
       <c r="E36" s="37"/>
@@ -6141,16 +6163,16 @@
       <c r="Y36" s="6"/>
     </row>
     <row r="37" spans="1:25" ht="14.25" customHeight="1">
-      <c r="A37" s="40" t="s">
-        <v>209</v>
-      </c>
-      <c r="B37" s="41"/>
-      <c r="C37" s="41"/>
+      <c r="A37" s="39" t="s">
+        <v>199</v>
+      </c>
+      <c r="B37" s="40"/>
+      <c r="C37" s="40"/>
       <c r="D37" s="13" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="E37" s="13" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
@@ -6176,14 +6198,14 @@
     <row r="38" spans="1:25" ht="14.25" customHeight="1">
       <c r="A38" s="18"/>
       <c r="B38" s="36" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
       <c r="C38" s="37"/>
       <c r="D38" s="38" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="E38" s="38" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
@@ -6210,7 +6232,7 @@
       <c r="A39" s="18"/>
       <c r="B39" s="18"/>
       <c r="C39" s="19" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="D39" s="37"/>
       <c r="E39" s="37"/>
@@ -6238,14 +6260,14 @@
     <row r="40" spans="1:25" ht="14.25" customHeight="1">
       <c r="A40" s="18"/>
       <c r="B40" s="36" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="C40" s="37"/>
       <c r="D40" s="38" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="E40" s="38" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
@@ -6272,7 +6294,7 @@
       <c r="A41" s="18"/>
       <c r="B41" s="18"/>
       <c r="C41" s="19" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
       <c r="D41" s="37"/>
       <c r="E41" s="37"/>
@@ -6300,14 +6322,14 @@
     <row r="42" spans="1:25" ht="14.25" customHeight="1">
       <c r="A42" s="18"/>
       <c r="B42" s="36" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="C42" s="37"/>
       <c r="D42" s="38" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="E42" s="38" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="F42" s="6"/>
       <c r="G42" s="6"/>
@@ -6334,7 +6356,7 @@
       <c r="A43" s="18"/>
       <c r="B43" s="18"/>
       <c r="C43" s="19" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="D43" s="37"/>
       <c r="E43" s="37"/>
@@ -6362,14 +6384,14 @@
     <row r="44" spans="1:25" ht="14.25" customHeight="1">
       <c r="A44" s="18"/>
       <c r="B44" s="36" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="C44" s="37"/>
       <c r="D44" s="38" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="E44" s="38" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
@@ -6396,7 +6418,7 @@
       <c r="A45" s="18"/>
       <c r="B45" s="18"/>
       <c r="C45" s="19" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="D45" s="37"/>
       <c r="E45" s="37"/>
@@ -6422,16 +6444,16 @@
       <c r="Y45" s="6"/>
     </row>
     <row r="46" spans="1:25" ht="14.25" customHeight="1">
-      <c r="A46" s="40" t="s">
-        <v>228</v>
-      </c>
-      <c r="B46" s="41"/>
-      <c r="C46" s="41"/>
+      <c r="A46" s="39" t="s">
+        <v>218</v>
+      </c>
+      <c r="B46" s="40"/>
+      <c r="C46" s="40"/>
       <c r="D46" s="13" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="E46" s="13" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
@@ -6457,14 +6479,14 @@
     <row r="47" spans="1:25" ht="14.25" customHeight="1">
       <c r="A47" s="18"/>
       <c r="B47" s="36" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
       <c r="C47" s="37"/>
       <c r="D47" s="38" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="E47" s="38" t="s">
-        <v>233</v>
+        <v>223</v>
       </c>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
@@ -6491,7 +6513,7 @@
       <c r="A48" s="18"/>
       <c r="B48" s="18"/>
       <c r="C48" s="19" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
       <c r="D48" s="37"/>
       <c r="E48" s="37"/>
@@ -6519,14 +6541,14 @@
     <row r="49" spans="1:25" ht="14.25" customHeight="1">
       <c r="A49" s="18"/>
       <c r="B49" s="36" t="s">
-        <v>235</v>
+        <v>225</v>
       </c>
       <c r="C49" s="37"/>
       <c r="D49" s="38" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
       <c r="E49" s="38" t="s">
-        <v>237</v>
+        <v>227</v>
       </c>
       <c r="F49" s="6"/>
       <c r="G49" s="6"/>
@@ -6553,7 +6575,7 @@
       <c r="A50" s="18"/>
       <c r="B50" s="18"/>
       <c r="C50" s="19" t="s">
-        <v>238</v>
+        <v>228</v>
       </c>
       <c r="D50" s="37"/>
       <c r="E50" s="37"/>
@@ -6581,14 +6603,14 @@
     <row r="51" spans="1:25" ht="14.25" customHeight="1">
       <c r="A51" s="18"/>
       <c r="B51" s="36" t="s">
-        <v>239</v>
+        <v>229</v>
       </c>
       <c r="C51" s="37"/>
       <c r="D51" s="38" t="s">
-        <v>240</v>
+        <v>230</v>
       </c>
       <c r="E51" s="38" t="s">
-        <v>241</v>
+        <v>231</v>
       </c>
       <c r="F51" s="6"/>
       <c r="G51" s="6"/>
@@ -6615,7 +6637,7 @@
       <c r="A52" s="18"/>
       <c r="B52" s="18"/>
       <c r="C52" s="19" t="s">
-        <v>242</v>
+        <v>232</v>
       </c>
       <c r="D52" s="37"/>
       <c r="E52" s="37"/>
@@ -6641,16 +6663,16 @@
       <c r="Y52" s="6"/>
     </row>
     <row r="53" spans="1:25" ht="14.25" customHeight="1">
-      <c r="A53" s="40" t="s">
-        <v>243</v>
-      </c>
-      <c r="B53" s="41"/>
-      <c r="C53" s="41"/>
+      <c r="A53" s="39" t="s">
+        <v>233</v>
+      </c>
+      <c r="B53" s="40"/>
+      <c r="C53" s="40"/>
       <c r="D53" s="13" t="s">
-        <v>244</v>
+        <v>234</v>
       </c>
       <c r="E53" s="13" t="s">
-        <v>245</v>
+        <v>235</v>
       </c>
       <c r="F53" s="6"/>
       <c r="G53" s="6"/>
@@ -6676,14 +6698,14 @@
     <row r="54" spans="1:25" ht="14.25" customHeight="1">
       <c r="A54" s="18"/>
       <c r="B54" s="36" t="s">
-        <v>246</v>
+        <v>236</v>
       </c>
       <c r="C54" s="37"/>
       <c r="D54" s="38" t="s">
-        <v>247</v>
+        <v>237</v>
       </c>
       <c r="E54" s="38" t="s">
-        <v>248</v>
+        <v>238</v>
       </c>
       <c r="F54" s="6"/>
       <c r="G54" s="6"/>
@@ -6710,7 +6732,7 @@
       <c r="A55" s="18"/>
       <c r="B55" s="18"/>
       <c r="C55" s="19" t="s">
-        <v>249</v>
+        <v>239</v>
       </c>
       <c r="D55" s="37"/>
       <c r="E55" s="37"/>
@@ -6738,14 +6760,14 @@
     <row r="56" spans="1:25" ht="14.25" customHeight="1">
       <c r="A56" s="18"/>
       <c r="B56" s="36" t="s">
-        <v>250</v>
+        <v>240</v>
       </c>
       <c r="C56" s="37"/>
       <c r="D56" s="38" t="s">
-        <v>251</v>
+        <v>241</v>
       </c>
       <c r="E56" s="38" t="s">
-        <v>252</v>
+        <v>242</v>
       </c>
       <c r="F56" s="6"/>
       <c r="G56" s="6"/>
@@ -6772,7 +6794,7 @@
       <c r="A57" s="18"/>
       <c r="B57" s="18"/>
       <c r="C57" s="19" t="s">
-        <v>253</v>
+        <v>243</v>
       </c>
       <c r="D57" s="37"/>
       <c r="E57" s="37"/>
@@ -6800,11 +6822,11 @@
     <row r="58" spans="1:25" ht="14.25" customHeight="1">
       <c r="A58" s="18"/>
       <c r="B58" s="36" t="s">
-        <v>254</v>
+        <v>244</v>
       </c>
       <c r="C58" s="37"/>
       <c r="D58" s="38" t="s">
-        <v>255</v>
+        <v>245</v>
       </c>
       <c r="E58" s="38"/>
       <c r="F58" s="6"/>
@@ -6832,7 +6854,7 @@
       <c r="A59" s="18"/>
       <c r="B59" s="18"/>
       <c r="C59" s="19" t="s">
-        <v>256</v>
+        <v>246</v>
       </c>
       <c r="D59" s="37"/>
       <c r="E59" s="37"/>
@@ -6858,16 +6880,16 @@
       <c r="Y59" s="6"/>
     </row>
     <row r="60" spans="1:25" ht="14.25" customHeight="1">
-      <c r="A60" s="40" t="s">
-        <v>257</v>
-      </c>
-      <c r="B60" s="41"/>
-      <c r="C60" s="41"/>
+      <c r="A60" s="39" t="s">
+        <v>247</v>
+      </c>
+      <c r="B60" s="40"/>
+      <c r="C60" s="40"/>
       <c r="D60" s="13" t="s">
-        <v>258</v>
+        <v>248</v>
       </c>
       <c r="E60" s="13" t="s">
-        <v>259</v>
+        <v>249</v>
       </c>
       <c r="F60" s="6"/>
       <c r="G60" s="6"/>
@@ -6893,14 +6915,14 @@
     <row r="61" spans="1:25" ht="14.25" customHeight="1">
       <c r="A61" s="18"/>
       <c r="B61" s="36" t="s">
-        <v>260</v>
+        <v>250</v>
       </c>
       <c r="C61" s="37"/>
       <c r="D61" s="38" t="s">
-        <v>261</v>
+        <v>251</v>
       </c>
       <c r="E61" s="38" t="s">
-        <v>262</v>
+        <v>252</v>
       </c>
       <c r="F61" s="6"/>
       <c r="G61" s="6"/>
@@ -6927,7 +6949,7 @@
       <c r="A62" s="18"/>
       <c r="B62" s="18"/>
       <c r="C62" s="19" t="s">
-        <v>263</v>
+        <v>253</v>
       </c>
       <c r="D62" s="37"/>
       <c r="E62" s="37"/>
@@ -6955,14 +6977,14 @@
     <row r="63" spans="1:25" ht="14.25" customHeight="1">
       <c r="A63" s="18"/>
       <c r="B63" s="36" t="s">
-        <v>264</v>
+        <v>254</v>
       </c>
       <c r="C63" s="37"/>
       <c r="D63" s="38" t="s">
-        <v>265</v>
+        <v>255</v>
       </c>
       <c r="E63" s="38" t="s">
-        <v>266</v>
+        <v>256</v>
       </c>
       <c r="F63" s="6"/>
       <c r="G63" s="6"/>
@@ -6989,7 +7011,7 @@
       <c r="A64" s="18"/>
       <c r="B64" s="18"/>
       <c r="C64" s="19" t="s">
-        <v>267</v>
+        <v>257</v>
       </c>
       <c r="D64" s="37"/>
       <c r="E64" s="37"/>
@@ -7017,14 +7039,14 @@
     <row r="65" spans="1:25" ht="14.25" customHeight="1">
       <c r="A65" s="18"/>
       <c r="B65" s="36" t="s">
-        <v>268</v>
+        <v>258</v>
       </c>
       <c r="C65" s="37"/>
       <c r="D65" s="38" t="s">
-        <v>269</v>
+        <v>259</v>
       </c>
       <c r="E65" s="38" t="s">
-        <v>270</v>
+        <v>260</v>
       </c>
       <c r="F65" s="6"/>
       <c r="G65" s="6"/>
@@ -7051,7 +7073,7 @@
       <c r="A66" s="18"/>
       <c r="B66" s="18"/>
       <c r="C66" s="19" t="s">
-        <v>271</v>
+        <v>261</v>
       </c>
       <c r="D66" s="37"/>
       <c r="E66" s="37"/>
@@ -7077,16 +7099,16 @@
       <c r="Y66" s="6"/>
     </row>
     <row r="67" spans="1:25" ht="14.25" customHeight="1">
-      <c r="A67" s="40" t="s">
-        <v>272</v>
-      </c>
-      <c r="B67" s="41"/>
-      <c r="C67" s="41"/>
+      <c r="A67" s="39" t="s">
+        <v>262</v>
+      </c>
+      <c r="B67" s="40"/>
+      <c r="C67" s="40"/>
       <c r="D67" s="13" t="s">
-        <v>273</v>
+        <v>263</v>
       </c>
       <c r="E67" s="13" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="F67" s="6"/>
       <c r="G67" s="6"/>
@@ -7112,14 +7134,14 @@
     <row r="68" spans="1:25" ht="14.25" customHeight="1">
       <c r="A68" s="18"/>
       <c r="B68" s="36" t="s">
-        <v>275</v>
+        <v>265</v>
       </c>
       <c r="C68" s="37"/>
       <c r="D68" s="38" t="s">
-        <v>276</v>
+        <v>266</v>
       </c>
       <c r="E68" s="38" t="s">
-        <v>277</v>
+        <v>267</v>
       </c>
       <c r="F68" s="6"/>
       <c r="G68" s="6"/>
@@ -7146,7 +7168,7 @@
       <c r="A69" s="18"/>
       <c r="B69" s="18"/>
       <c r="C69" s="19" t="s">
-        <v>278</v>
+        <v>268</v>
       </c>
       <c r="D69" s="37"/>
       <c r="E69" s="37"/>
@@ -7174,14 +7196,14 @@
     <row r="70" spans="1:25" ht="14.25" customHeight="1">
       <c r="A70" s="18"/>
       <c r="B70" s="36" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
       <c r="C70" s="37"/>
       <c r="D70" s="38" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="E70" s="38" t="s">
-        <v>281</v>
+        <v>271</v>
       </c>
       <c r="F70" s="6"/>
       <c r="G70" s="6"/>
@@ -7208,7 +7230,7 @@
       <c r="A71" s="18"/>
       <c r="B71" s="18"/>
       <c r="C71" s="19" t="s">
-        <v>282</v>
+        <v>272</v>
       </c>
       <c r="D71" s="37"/>
       <c r="E71" s="37"/>
@@ -7236,14 +7258,14 @@
     <row r="72" spans="1:25" ht="14.25" customHeight="1">
       <c r="A72" s="18"/>
       <c r="B72" s="36" t="s">
-        <v>283</v>
+        <v>273</v>
       </c>
       <c r="C72" s="37"/>
       <c r="D72" s="38" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
       <c r="E72" s="38" t="s">
-        <v>285</v>
+        <v>275</v>
       </c>
       <c r="F72" s="6"/>
       <c r="G72" s="6"/>
@@ -7270,7 +7292,7 @@
       <c r="A73" s="18"/>
       <c r="B73" s="18"/>
       <c r="C73" s="19" t="s">
-        <v>286</v>
+        <v>276</v>
       </c>
       <c r="D73" s="37"/>
       <c r="E73" s="37"/>
@@ -7298,14 +7320,14 @@
     <row r="74" spans="1:25" ht="14.25" customHeight="1">
       <c r="A74" s="18"/>
       <c r="B74" s="36" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
       <c r="C74" s="37"/>
       <c r="D74" s="38" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="E74" s="38" t="s">
-        <v>289</v>
+        <v>279</v>
       </c>
       <c r="F74" s="6"/>
       <c r="G74" s="6"/>
@@ -7332,7 +7354,7 @@
       <c r="A75" s="18"/>
       <c r="B75" s="18"/>
       <c r="C75" s="19" t="s">
-        <v>290</v>
+        <v>280</v>
       </c>
       <c r="D75" s="37"/>
       <c r="E75" s="37"/>
@@ -7360,14 +7382,14 @@
     <row r="76" spans="1:25" ht="14.25" customHeight="1">
       <c r="A76" s="18"/>
       <c r="B76" s="36" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="C76" s="37"/>
       <c r="D76" s="38" t="s">
-        <v>292</v>
+        <v>282</v>
       </c>
       <c r="E76" s="38" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
       <c r="F76" s="6"/>
       <c r="G76" s="6"/>
@@ -7394,7 +7416,7 @@
       <c r="A77" s="18"/>
       <c r="B77" s="18"/>
       <c r="C77" s="19" t="s">
-        <v>294</v>
+        <v>284</v>
       </c>
       <c r="D77" s="37"/>
       <c r="E77" s="37"/>
@@ -7422,14 +7444,14 @@
     <row r="78" spans="1:25" ht="14.25" customHeight="1">
       <c r="A78" s="18"/>
       <c r="B78" s="36" t="s">
-        <v>295</v>
+        <v>285</v>
       </c>
       <c r="C78" s="37"/>
       <c r="D78" s="38" t="s">
-        <v>296</v>
+        <v>286</v>
       </c>
       <c r="E78" s="38" t="s">
-        <v>297</v>
+        <v>287</v>
       </c>
       <c r="F78" s="6"/>
       <c r="G78" s="6"/>
@@ -7456,7 +7478,7 @@
       <c r="A79" s="18"/>
       <c r="B79" s="18"/>
       <c r="C79" s="19" t="s">
-        <v>298</v>
+        <v>288</v>
       </c>
       <c r="D79" s="37"/>
       <c r="E79" s="37"/>
@@ -7482,16 +7504,16 @@
       <c r="Y79" s="6"/>
     </row>
     <row r="80" spans="1:25" ht="14.25" customHeight="1">
-      <c r="A80" s="40" t="s">
-        <v>299</v>
-      </c>
-      <c r="B80" s="41"/>
-      <c r="C80" s="41"/>
+      <c r="A80" s="39" t="s">
+        <v>289</v>
+      </c>
+      <c r="B80" s="40"/>
+      <c r="C80" s="40"/>
       <c r="D80" s="13" t="s">
-        <v>300</v>
+        <v>290</v>
       </c>
       <c r="E80" s="13" t="s">
-        <v>301</v>
+        <v>291</v>
       </c>
       <c r="F80" s="6"/>
       <c r="G80" s="6"/>
@@ -7517,11 +7539,11 @@
     <row r="81" spans="1:25" ht="14.25" customHeight="1">
       <c r="A81" s="18"/>
       <c r="B81" s="36" t="s">
-        <v>302</v>
+        <v>292</v>
       </c>
       <c r="C81" s="37"/>
       <c r="D81" s="38" t="s">
-        <v>303</v>
+        <v>293</v>
       </c>
       <c r="E81" s="38"/>
       <c r="F81" s="6"/>
@@ -7549,7 +7571,7 @@
       <c r="A82" s="18"/>
       <c r="B82" s="18"/>
       <c r="C82" s="19" t="s">
-        <v>304</v>
+        <v>294</v>
       </c>
       <c r="D82" s="37"/>
       <c r="E82" s="37"/>
@@ -7577,11 +7599,11 @@
     <row r="83" spans="1:25" ht="14.25" customHeight="1">
       <c r="A83" s="18"/>
       <c r="B83" s="36" t="s">
-        <v>305</v>
+        <v>295</v>
       </c>
       <c r="C83" s="37"/>
       <c r="D83" s="38" t="s">
-        <v>306</v>
+        <v>296</v>
       </c>
       <c r="E83" s="38"/>
       <c r="F83" s="6"/>
@@ -7609,7 +7631,7 @@
       <c r="A84" s="18"/>
       <c r="B84" s="18"/>
       <c r="C84" s="19" t="s">
-        <v>307</v>
+        <v>297</v>
       </c>
       <c r="D84" s="37"/>
       <c r="E84" s="37"/>
@@ -7637,11 +7659,11 @@
     <row r="85" spans="1:25" ht="14.25" customHeight="1">
       <c r="A85" s="18"/>
       <c r="B85" s="36" t="s">
-        <v>308</v>
+        <v>298</v>
       </c>
       <c r="C85" s="37"/>
       <c r="D85" s="38" t="s">
-        <v>309</v>
+        <v>299</v>
       </c>
       <c r="E85" s="38"/>
       <c r="F85" s="6"/>
@@ -7669,7 +7691,7 @@
       <c r="A86" s="18"/>
       <c r="B86" s="18"/>
       <c r="C86" s="19" t="s">
-        <v>310</v>
+        <v>300</v>
       </c>
       <c r="D86" s="37"/>
       <c r="E86" s="37"/>
@@ -7695,16 +7717,16 @@
       <c r="Y86" s="6"/>
     </row>
     <row r="87" spans="1:25" ht="14.25" customHeight="1">
-      <c r="A87" s="40" t="s">
-        <v>311</v>
-      </c>
-      <c r="B87" s="41"/>
-      <c r="C87" s="41"/>
+      <c r="A87" s="39" t="s">
+        <v>301</v>
+      </c>
+      <c r="B87" s="40"/>
+      <c r="C87" s="40"/>
       <c r="D87" s="13" t="s">
-        <v>312</v>
+        <v>302</v>
       </c>
       <c r="E87" s="13" t="s">
-        <v>313</v>
+        <v>303</v>
       </c>
       <c r="F87" s="6"/>
       <c r="G87" s="6"/>
@@ -7730,14 +7752,14 @@
     <row r="88" spans="1:25" ht="14.25" customHeight="1">
       <c r="A88" s="18"/>
       <c r="B88" s="36" t="s">
-        <v>314</v>
+        <v>304</v>
       </c>
       <c r="C88" s="37"/>
       <c r="D88" s="38" t="s">
-        <v>315</v>
+        <v>305</v>
       </c>
       <c r="E88" s="38" t="s">
-        <v>316</v>
+        <v>306</v>
       </c>
       <c r="F88" s="6"/>
       <c r="G88" s="6"/>
@@ -7764,7 +7786,7 @@
       <c r="A89" s="18"/>
       <c r="B89" s="18"/>
       <c r="C89" s="19" t="s">
-        <v>317</v>
+        <v>307</v>
       </c>
       <c r="D89" s="37"/>
       <c r="E89" s="37"/>
@@ -7792,11 +7814,11 @@
     <row r="90" spans="1:25" ht="14.25" customHeight="1">
       <c r="A90" s="18"/>
       <c r="B90" s="36" t="s">
-        <v>318</v>
+        <v>308</v>
       </c>
       <c r="C90" s="37"/>
       <c r="D90" s="38" t="s">
-        <v>319</v>
+        <v>309</v>
       </c>
       <c r="E90" s="38"/>
       <c r="F90" s="6"/>
@@ -7824,7 +7846,7 @@
       <c r="A91" s="18"/>
       <c r="B91" s="18"/>
       <c r="C91" s="19" t="s">
-        <v>320</v>
+        <v>310</v>
       </c>
       <c r="D91" s="37"/>
       <c r="E91" s="37"/>
@@ -7852,11 +7874,11 @@
     <row r="92" spans="1:25" ht="14.25" customHeight="1">
       <c r="A92" s="18"/>
       <c r="B92" s="36" t="s">
-        <v>321</v>
+        <v>311</v>
       </c>
       <c r="C92" s="37"/>
       <c r="D92" s="38" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
       <c r="E92" s="38"/>
       <c r="F92" s="6"/>
@@ -7884,7 +7906,7 @@
       <c r="A93" s="18"/>
       <c r="B93" s="18"/>
       <c r="C93" s="19" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="D93" s="37"/>
       <c r="E93" s="37"/>
@@ -7912,11 +7934,11 @@
     <row r="94" spans="1:25" ht="14.25" customHeight="1">
       <c r="A94" s="18"/>
       <c r="B94" s="36" t="s">
-        <v>324</v>
+        <v>314</v>
       </c>
       <c r="C94" s="37"/>
       <c r="D94" s="38" t="s">
-        <v>325</v>
+        <v>315</v>
       </c>
       <c r="E94" s="38"/>
       <c r="F94" s="6"/>
@@ -7944,10 +7966,10 @@
       <c r="A95" s="20"/>
       <c r="B95" s="20"/>
       <c r="C95" s="21" t="s">
-        <v>326</v>
-      </c>
-      <c r="D95" s="39"/>
-      <c r="E95" s="39"/>
+        <v>316</v>
+      </c>
+      <c r="D95" s="41"/>
+      <c r="E95" s="41"/>
       <c r="F95" s="6"/>
       <c r="G95" s="6"/>
       <c r="H95" s="6"/>
@@ -14076,6 +14098,123 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="131">
+    <mergeCell ref="B92:C92"/>
+    <mergeCell ref="D92:D93"/>
+    <mergeCell ref="E92:E93"/>
+    <mergeCell ref="B94:C94"/>
+    <mergeCell ref="D94:D95"/>
+    <mergeCell ref="E94:E95"/>
+    <mergeCell ref="A87:C87"/>
+    <mergeCell ref="B88:C88"/>
+    <mergeCell ref="D88:D89"/>
+    <mergeCell ref="E88:E89"/>
+    <mergeCell ref="B90:C90"/>
+    <mergeCell ref="D90:D91"/>
+    <mergeCell ref="E90:E91"/>
+    <mergeCell ref="B83:C83"/>
+    <mergeCell ref="D83:D84"/>
+    <mergeCell ref="E83:E84"/>
+    <mergeCell ref="B85:C85"/>
+    <mergeCell ref="D85:D86"/>
+    <mergeCell ref="E85:E86"/>
+    <mergeCell ref="B78:C78"/>
+    <mergeCell ref="D78:D79"/>
+    <mergeCell ref="E78:E79"/>
+    <mergeCell ref="A80:C80"/>
+    <mergeCell ref="B81:C81"/>
+    <mergeCell ref="D81:D82"/>
+    <mergeCell ref="E81:E82"/>
+    <mergeCell ref="B74:C74"/>
+    <mergeCell ref="D74:D75"/>
+    <mergeCell ref="E74:E75"/>
+    <mergeCell ref="B76:C76"/>
+    <mergeCell ref="D76:D77"/>
+    <mergeCell ref="E76:E77"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="D70:D71"/>
+    <mergeCell ref="E70:E71"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="D72:D73"/>
+    <mergeCell ref="E72:E73"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="D65:D66"/>
+    <mergeCell ref="E65:E66"/>
+    <mergeCell ref="A67:C67"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="D68:D69"/>
+    <mergeCell ref="E68:E69"/>
+    <mergeCell ref="A60:C60"/>
+    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="D61:D62"/>
+    <mergeCell ref="E61:E62"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="D63:D64"/>
+    <mergeCell ref="E63:E64"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="D56:D57"/>
+    <mergeCell ref="E56:E57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="D58:D59"/>
+    <mergeCell ref="E58:E59"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="D51:D52"/>
+    <mergeCell ref="E51:E52"/>
+    <mergeCell ref="A53:C53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="D54:D55"/>
+    <mergeCell ref="E54:E55"/>
+    <mergeCell ref="A46:C46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="D47:D48"/>
+    <mergeCell ref="E47:E48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="D49:D50"/>
+    <mergeCell ref="E49:E50"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="E42:E43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="E44:E45"/>
+    <mergeCell ref="A37:C37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="E38:E39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="D40:D41"/>
+    <mergeCell ref="E40:E41"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="E33:E34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="E35:E36"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E17:E18"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="D10:D11"/>
     <mergeCell ref="E10:E11"/>
@@ -14090,123 +14229,6 @@
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="D8:D9"/>
     <mergeCell ref="E8:E9"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="A28:C28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="E31:E32"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="A37:C37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="E38:E39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="D40:D41"/>
-    <mergeCell ref="E40:E41"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="E33:E34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="E35:E36"/>
-    <mergeCell ref="A46:C46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="D47:D48"/>
-    <mergeCell ref="E47:E48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="D49:D50"/>
-    <mergeCell ref="E49:E50"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="D42:D43"/>
-    <mergeCell ref="E42:E43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="D44:D45"/>
-    <mergeCell ref="E44:E45"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="D56:D57"/>
-    <mergeCell ref="E56:E57"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="D58:D59"/>
-    <mergeCell ref="E58:E59"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="D51:D52"/>
-    <mergeCell ref="E51:E52"/>
-    <mergeCell ref="A53:C53"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="D54:D55"/>
-    <mergeCell ref="E54:E55"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="D65:D66"/>
-    <mergeCell ref="E65:E66"/>
-    <mergeCell ref="A67:C67"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="D68:D69"/>
-    <mergeCell ref="E68:E69"/>
-    <mergeCell ref="A60:C60"/>
-    <mergeCell ref="B61:C61"/>
-    <mergeCell ref="D61:D62"/>
-    <mergeCell ref="E61:E62"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="D63:D64"/>
-    <mergeCell ref="E63:E64"/>
-    <mergeCell ref="B74:C74"/>
-    <mergeCell ref="D74:D75"/>
-    <mergeCell ref="E74:E75"/>
-    <mergeCell ref="B76:C76"/>
-    <mergeCell ref="D76:D77"/>
-    <mergeCell ref="E76:E77"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="D70:D71"/>
-    <mergeCell ref="E70:E71"/>
-    <mergeCell ref="B72:C72"/>
-    <mergeCell ref="D72:D73"/>
-    <mergeCell ref="E72:E73"/>
-    <mergeCell ref="B83:C83"/>
-    <mergeCell ref="D83:D84"/>
-    <mergeCell ref="E83:E84"/>
-    <mergeCell ref="B85:C85"/>
-    <mergeCell ref="D85:D86"/>
-    <mergeCell ref="E85:E86"/>
-    <mergeCell ref="B78:C78"/>
-    <mergeCell ref="D78:D79"/>
-    <mergeCell ref="E78:E79"/>
-    <mergeCell ref="A80:C80"/>
-    <mergeCell ref="B81:C81"/>
-    <mergeCell ref="D81:D82"/>
-    <mergeCell ref="E81:E82"/>
-    <mergeCell ref="B92:C92"/>
-    <mergeCell ref="D92:D93"/>
-    <mergeCell ref="E92:E93"/>
-    <mergeCell ref="B94:C94"/>
-    <mergeCell ref="D94:D95"/>
-    <mergeCell ref="E94:E95"/>
-    <mergeCell ref="A87:C87"/>
-    <mergeCell ref="B88:C88"/>
-    <mergeCell ref="D88:D89"/>
-    <mergeCell ref="E88:E89"/>
-    <mergeCell ref="B90:C90"/>
-    <mergeCell ref="D90:D91"/>
-    <mergeCell ref="E90:E91"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1"/>

</xml_diff>

<commit_message>
change authors to report_writers
</commit_message>
<xml_diff>
--- a/data-raw/data-out/CAN-SARD_data_dictionary.xlsx
+++ b/data-raw/data-out/CAN-SARD_data_dictionary.xlsx
@@ -104,9 +104,6 @@
   </si>
   <si>
     <t>continuous_USA</t>
-  </si>
-  <si>
-    <t>author</t>
   </si>
   <si>
     <t>Smith, J.</t>
@@ -2007,9 +2004,6 @@
     <t>Extracted from SAR Data Management System under 'Legal List' or from the status report</t>
   </si>
   <si>
-    <t xml:space="preserve">Last names and first initials for status report authors </t>
-  </si>
-  <si>
     <t>NA if not a status report</t>
   </si>
   <si>
@@ -2275,6 +2269,12 @@
   </si>
   <si>
     <t xml:space="preserve"> Vascular Plants</t>
+  </si>
+  <si>
+    <t>report_writers</t>
+  </si>
+  <si>
+    <t>Last names and first initials for status report writers</t>
   </si>
 </sst>
 </file>
@@ -2556,11 +2556,11 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2974,8 +2974,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2998,7 +2998,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="23" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D1" s="34" t="s">
         <v>2</v>
@@ -3017,13 +3017,13 @@
     </row>
     <row r="2" spans="1:15">
       <c r="A2" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="D2" s="27" t="s">
         <v>20</v>
@@ -3042,13 +3042,13 @@
     </row>
     <row r="3" spans="1:15" ht="28.8">
       <c r="A3" s="1" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="D3" s="25" t="s">
         <v>20</v>
@@ -3070,10 +3070,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="D4" s="25" t="s">
         <v>4</v>
@@ -3098,7 +3098,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="D5" s="25" t="s">
         <v>4</v>
@@ -3117,22 +3117,22 @@
     </row>
     <row r="6" spans="1:15" ht="28.8">
       <c r="A6" s="1" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B6" s="27" t="s">
+        <v>373</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>375</v>
-      </c>
       <c r="D6" s="24" t="s">
+        <v>370</v>
+      </c>
+      <c r="E6" s="26" t="s">
         <v>371</v>
       </c>
-      <c r="E6" s="26" t="s">
+      <c r="F6" s="26" t="s">
         <v>372</v>
-      </c>
-      <c r="F6" s="26" t="s">
-        <v>373</v>
       </c>
       <c r="G6" s="26"/>
       <c r="H6" s="26"/>
@@ -3152,7 +3152,7 @@
         <v>13</v>
       </c>
       <c r="C7" s="29" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D7" s="25" t="s">
         <v>8</v>
@@ -3175,13 +3175,13 @@
     </row>
     <row r="8" spans="1:15">
       <c r="A8" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B8" s="29" t="s">
+        <v>375</v>
+      </c>
+      <c r="C8" s="29" t="s">
         <v>376</v>
-      </c>
-      <c r="C8" s="29" t="s">
-        <v>377</v>
       </c>
       <c r="D8" s="25"/>
       <c r="E8" s="25"/>
@@ -3198,16 +3198,16 @@
     </row>
     <row r="9" spans="1:15" ht="28.8">
       <c r="A9" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B9" s="29" t="s">
+        <v>378</v>
+      </c>
+      <c r="C9" s="29" t="s">
         <v>379</v>
       </c>
-      <c r="C9" s="29" t="s">
-        <v>380</v>
-      </c>
       <c r="D9" s="27" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="E9" s="25"/>
       <c r="F9" s="25"/>
@@ -3223,13 +3223,13 @@
     </row>
     <row r="10" spans="1:15">
       <c r="A10" s="1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>381</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>382</v>
       </c>
       <c r="D10" s="25" t="s">
         <v>7</v>
@@ -3248,16 +3248,16 @@
     </row>
     <row r="11" spans="1:15" ht="28.8">
       <c r="A11" s="1" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="D11" s="27" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="E11" s="25"/>
       <c r="F11" s="25"/>
@@ -3273,10 +3273,10 @@
     </row>
     <row r="12" spans="1:15" ht="28.8">
       <c r="A12" s="1" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="25" t="s">
@@ -3292,13 +3292,13 @@
     </row>
     <row r="13" spans="1:15" ht="43.2">
       <c r="A13" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>385</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>386</v>
       </c>
       <c r="D13" s="25" t="s">
         <v>14</v>
@@ -3317,13 +3317,13 @@
     </row>
     <row r="14" spans="1:15" ht="28.8">
       <c r="A14" s="1" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>387</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>388</v>
       </c>
       <c r="D14" s="25" t="s">
         <v>14</v>
@@ -3342,64 +3342,64 @@
     </row>
     <row r="15" spans="1:15">
       <c r="A15" s="1" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="25" t="s">
+        <v>468</v>
+      </c>
+      <c r="E15" s="25" t="s">
+        <v>469</v>
+      </c>
+      <c r="F15" s="25" t="s">
         <v>470</v>
       </c>
-      <c r="E15" s="25" t="s">
+      <c r="G15" s="25" t="s">
         <v>471</v>
       </c>
-      <c r="F15" s="25" t="s">
+      <c r="H15" s="25" t="s">
         <v>472</v>
       </c>
-      <c r="G15" s="25" t="s">
+      <c r="I15" s="25" t="s">
         <v>473</v>
       </c>
-      <c r="H15" s="25" t="s">
+      <c r="J15" s="25" t="s">
         <v>474</v>
       </c>
-      <c r="I15" s="25" t="s">
+      <c r="K15" s="25" t="s">
         <v>475</v>
       </c>
-      <c r="J15" s="25" t="s">
+      <c r="L15" s="25" t="s">
         <v>476</v>
       </c>
-      <c r="K15" s="25" t="s">
+      <c r="M15" s="25" t="s">
         <v>477</v>
       </c>
-      <c r="L15" s="25" t="s">
+      <c r="N15" s="25" t="s">
         <v>478</v>
       </c>
-      <c r="M15" s="25" t="s">
+      <c r="O15" s="25" t="s">
         <v>479</v>
-      </c>
-      <c r="N15" s="25" t="s">
-        <v>480</v>
-      </c>
-      <c r="O15" s="25" t="s">
-        <v>481</v>
       </c>
     </row>
     <row r="16" spans="1:15" ht="28.8">
       <c r="A16" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>481</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D16" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>392</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D16" s="25" t="s">
-        <v>27</v>
-      </c>
       <c r="E16" s="27" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="F16" s="25"/>
       <c r="G16" s="25"/>
@@ -3419,16 +3419,16 @@
         <v>16</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D17" s="24" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E17" s="27" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F17" s="27" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="G17" s="25"/>
       <c r="H17" s="25"/>
@@ -3450,16 +3450,16 @@
         <v>18</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D18" s="24" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E18" s="27" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F18" s="27" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="G18" s="25"/>
       <c r="H18" s="25"/>
@@ -3476,19 +3476,19 @@
         <v>19</v>
       </c>
       <c r="B19" s="27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D19" s="27" t="s">
         <v>20</v>
       </c>
       <c r="E19" s="27" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F19" s="27" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="G19" s="25"/>
       <c r="H19" s="25"/>
@@ -3508,13 +3508,13 @@
         <v>22</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D20" s="25" t="s">
         <v>14</v>
       </c>
       <c r="E20" s="27" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="F20" s="27"/>
       <c r="G20" s="25"/>
@@ -3535,13 +3535,13 @@
         <v>24</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D21" s="25" t="s">
         <v>14</v>
       </c>
       <c r="E21" s="27" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="F21" s="27"/>
       <c r="G21" s="25"/>
@@ -3559,16 +3559,16 @@
         <v>25</v>
       </c>
       <c r="B22" s="27" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D22" s="25" t="s">
         <v>14</v>
       </c>
       <c r="E22" s="27" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="F22" s="27"/>
       <c r="G22" s="25"/>
@@ -3583,13 +3583,13 @@
     </row>
     <row r="23" spans="1:17">
       <c r="A23" s="1" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B23" s="29" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="C23" s="29" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D23" s="25" t="s">
         <v>8</v>
@@ -3604,10 +3604,10 @@
         <v>11</v>
       </c>
       <c r="H23" s="27" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I23" s="25" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="J23" s="25"/>
       <c r="K23" s="25"/>
@@ -3617,16 +3617,16 @@
     </row>
     <row r="24" spans="1:17" ht="72">
       <c r="A24" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B24" s="24" t="s">
+        <v>389</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>390</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>391</v>
-      </c>
       <c r="D24" s="24" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="I24" s="25"/>
       <c r="K24" s="25"/>
@@ -3637,19 +3637,19 @@
     </row>
     <row r="25" spans="1:17" ht="57.6">
       <c r="A25" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D25" s="27" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="E25" s="27" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="F25" s="25"/>
       <c r="G25" s="25"/>
@@ -3664,19 +3664,19 @@
     </row>
     <row r="26" spans="1:17" ht="57.6">
       <c r="A26" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D26" s="27" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="E26" s="27" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="F26" s="25"/>
       <c r="G26" s="25"/>
@@ -3691,19 +3691,19 @@
     </row>
     <row r="27" spans="1:17" ht="57.6">
       <c r="A27" s="1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D27" s="27" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="E27" s="27" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="F27" s="25"/>
       <c r="G27" s="25"/>
@@ -3718,19 +3718,19 @@
     </row>
     <row r="28" spans="1:17" ht="57.6">
       <c r="A28" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D28" s="27" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="E28" s="27" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="F28" s="25"/>
       <c r="G28" s="25"/>
@@ -3745,19 +3745,19 @@
     </row>
     <row r="29" spans="1:17" ht="57.6">
       <c r="A29" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D29" s="27" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="E29" s="27" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="F29" s="25"/>
       <c r="G29" s="25"/>
@@ -3772,19 +3772,19 @@
     </row>
     <row r="30" spans="1:17" ht="57.6">
       <c r="A30" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B30" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="C30" s="1" t="s">
         <v>324</v>
       </c>
-      <c r="C30" s="1" t="s">
-        <v>325</v>
-      </c>
       <c r="D30" s="27" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="E30" s="27" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="F30" s="25"/>
       <c r="G30" s="25"/>
@@ -3799,28 +3799,28 @@
     </row>
     <row r="31" spans="1:17" ht="57.6">
       <c r="A31" s="1" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B31" s="27" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D31" s="25" t="s">
+        <v>395</v>
+      </c>
+      <c r="E31" s="25" t="s">
+        <v>396</v>
+      </c>
+      <c r="F31" s="25" t="s">
         <v>397</v>
       </c>
-      <c r="E31" s="25" t="s">
+      <c r="G31" s="25" t="s">
         <v>398</v>
       </c>
-      <c r="F31" s="25" t="s">
-        <v>399</v>
-      </c>
-      <c r="G31" s="25" t="s">
-        <v>400</v>
-      </c>
       <c r="H31" s="27" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="I31" s="25"/>
       <c r="J31" s="25"/>
@@ -3831,19 +3831,19 @@
     </row>
     <row r="32" spans="1:17" ht="100.8">
       <c r="A32" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C32" s="29" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="D32" s="26" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E32" s="27" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="F32" s="26"/>
       <c r="G32" s="26"/>
@@ -3858,19 +3858,19 @@
     </row>
     <row r="33" spans="1:15" ht="57.6">
       <c r="A33" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B33" s="24" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C33" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="D33" s="24" t="s">
         <v>112</v>
       </c>
-      <c r="D33" s="24" t="s">
-        <v>113</v>
-      </c>
       <c r="E33" s="27" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="L33" s="26"/>
       <c r="M33" s="26"/>
@@ -3879,13 +3879,13 @@
     </row>
     <row r="34" spans="1:15" ht="57.6">
       <c r="A34" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B34" s="24" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="D34" s="27" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="L34" s="26"/>
       <c r="M34" s="26"/>
@@ -3894,19 +3894,19 @@
     </row>
     <row r="35" spans="1:15" ht="57.6">
       <c r="A35" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B35" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="B35" s="24" t="s">
-        <v>78</v>
-      </c>
       <c r="C35" s="24" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D35" s="25" t="s">
         <v>14</v>
       </c>
       <c r="E35" s="27" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="L35" s="26"/>
       <c r="M35" s="26"/>
@@ -3915,19 +3915,19 @@
     </row>
     <row r="36" spans="1:15" ht="43.2">
       <c r="A36" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B36" s="24" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C36" s="29" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D36" s="24" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E36" s="24" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="L36" s="26"/>
       <c r="M36" s="26"/>
@@ -3936,13 +3936,13 @@
     </row>
     <row r="37" spans="1:15" ht="57.6">
       <c r="A37" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B37" s="24" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="D37" s="27" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="L37" s="26"/>
       <c r="M37" s="26"/>
@@ -3951,19 +3951,19 @@
     </row>
     <row r="38" spans="1:15" ht="28.8">
       <c r="A38" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B38" s="24" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C38" s="24" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D38" s="24" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E38" s="27" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="F38" s="25"/>
       <c r="G38" s="25"/>
@@ -3978,19 +3978,19 @@
     </row>
     <row r="39" spans="1:15" ht="43.2">
       <c r="A39" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B39" s="24" t="s">
         <v>114</v>
       </c>
-      <c r="B39" s="24" t="s">
-        <v>115</v>
-      </c>
       <c r="C39" s="29" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D39" s="24" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E39" s="24" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="F39" s="25"/>
       <c r="G39" s="25"/>
@@ -4005,13 +4005,13 @@
     </row>
     <row r="40" spans="1:15" ht="43.2">
       <c r="A40" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B40" s="27" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="C40" s="27" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="D40" s="25" t="s">
         <v>14</v>
@@ -4030,13 +4030,13 @@
     </row>
     <row r="41" spans="1:15" ht="72.599999999999994" thickBot="1">
       <c r="A41" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B41" s="27" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C41" s="27" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="D41" s="25" t="s">
         <v>14</v>
@@ -4055,13 +4055,13 @@
     </row>
     <row r="42" spans="1:15" ht="58.2" thickBot="1">
       <c r="A42" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B42" s="30" t="s">
+        <v>423</v>
+      </c>
+      <c r="C42" s="27" t="s">
         <v>425</v>
-      </c>
-      <c r="C42" s="27" t="s">
-        <v>427</v>
       </c>
       <c r="D42" s="27">
         <v>0</v>
@@ -4070,10 +4070,10 @@
         <v>1</v>
       </c>
       <c r="F42" s="27" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="G42" s="27" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="H42" s="25"/>
       <c r="I42" s="25"/>
@@ -4085,13 +4085,13 @@
     </row>
     <row r="43" spans="1:15" ht="101.4" thickBot="1">
       <c r="A43" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B43" s="31" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="C43" s="27" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="D43" s="27">
         <v>0</v>
@@ -4100,10 +4100,10 @@
         <v>1</v>
       </c>
       <c r="F43" s="27" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="G43" s="27" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="H43" s="26"/>
       <c r="I43" s="25"/>
@@ -4115,13 +4115,13 @@
     </row>
     <row r="44" spans="1:15" ht="101.4" thickBot="1">
       <c r="A44" s="1" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B44" s="31" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="C44" s="27" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="D44" s="27">
         <v>0</v>
@@ -4130,10 +4130,10 @@
         <v>1</v>
       </c>
       <c r="F44" s="27" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="G44" s="27" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="H44" s="26"/>
       <c r="I44" s="26"/>
@@ -4145,13 +4145,13 @@
     </row>
     <row r="45" spans="1:15" ht="101.4" thickBot="1">
       <c r="A45" s="1" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B45" s="31" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C45" s="27" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="D45" s="27">
         <v>0</v>
@@ -4160,21 +4160,21 @@
         <v>1</v>
       </c>
       <c r="F45" s="27" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="G45" s="27" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="46" spans="1:15" ht="101.4" thickBot="1">
       <c r="A46" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B46" s="31" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="C46" s="27" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="D46" s="27">
         <v>0</v>
@@ -4183,21 +4183,21 @@
         <v>1</v>
       </c>
       <c r="F46" s="27" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="G46" s="27" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="47" spans="1:15" ht="187.2">
       <c r="A47" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B47" s="27" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C47" s="27" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="D47" s="25" t="s">
         <v>14</v>
@@ -4207,43 +4207,43 @@
     </row>
     <row r="48" spans="1:15" ht="100.8">
       <c r="A48" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B48" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="C48" s="29" t="s">
+        <v>447</v>
+      </c>
+      <c r="D48" s="26" t="s">
         <v>119</v>
-      </c>
-      <c r="C48" s="29" t="s">
-        <v>449</v>
-      </c>
-      <c r="D48" s="26" t="s">
-        <v>120</v>
       </c>
       <c r="E48" s="27"/>
       <c r="F48" s="26"/>
     </row>
     <row r="49" spans="1:16" ht="28.8">
       <c r="A49" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B49" s="27" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="D49" s="25" t="s">
         <v>14</v>
       </c>
       <c r="E49" s="25" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="50" spans="1:16" ht="72">
       <c r="A50" s="1" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="D50" s="1">
         <v>1.1000000000000001</v>
@@ -4252,7 +4252,7 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="G50" s="1"/>
       <c r="H50" s="1"/>
@@ -4266,19 +4266,19 @@
     </row>
     <row r="51" spans="1:16" ht="28.8">
       <c r="A51" s="1" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B51" s="24" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="D51" s="24" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="G51" s="1"/>
       <c r="I51" s="1"/>
@@ -4292,19 +4292,19 @@
     </row>
     <row r="52" spans="1:16" ht="28.8">
       <c r="A52" s="1" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
@@ -4319,19 +4319,19 @@
     </row>
     <row r="53" spans="1:16" ht="28.8">
       <c r="A53" s="1" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B53" s="24" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="D53" s="24" t="s">
         <v>4</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="G53" s="1"/>
       <c r="I53" s="1"/>
@@ -4344,31 +4344,31 @@
     </row>
     <row r="54" spans="1:16" ht="28.8">
       <c r="A54" s="1" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E54" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="G54" s="1" t="s">
         <v>416</v>
       </c>
-      <c r="F54" s="1" t="s">
+      <c r="H54" s="1" t="s">
         <v>417</v>
       </c>
-      <c r="G54" s="1" t="s">
-        <v>418</v>
-      </c>
-      <c r="H54" s="1" t="s">
-        <v>419</v>
-      </c>
       <c r="I54" s="1" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="J54" s="26"/>
       <c r="K54" s="26"/>
@@ -4379,31 +4379,31 @@
     </row>
     <row r="55" spans="1:16" ht="28.8">
       <c r="A55" s="1" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B55" s="24" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="D55" s="24" t="s">
         <v>4</v>
       </c>
       <c r="E55" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="F55" s="24" t="s">
+        <v>415</v>
+      </c>
+      <c r="G55" s="1" t="s">
         <v>416</v>
       </c>
-      <c r="F55" s="24" t="s">
+      <c r="H55" s="24" t="s">
         <v>417</v>
       </c>
-      <c r="G55" s="1" t="s">
-        <v>418</v>
-      </c>
-      <c r="H55" s="24" t="s">
-        <v>419</v>
-      </c>
       <c r="I55" s="1" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="J55" s="26"/>
       <c r="K55" s="26"/>
@@ -4414,19 +4414,19 @@
     </row>
     <row r="56" spans="1:16" ht="28.8">
       <c r="A56" s="1" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="F56" s="1"/>
       <c r="G56" s="1"/>
@@ -4441,19 +4441,19 @@
     </row>
     <row r="57" spans="1:16" ht="28.8">
       <c r="A57" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B57" s="24" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="D57" s="24" t="s">
         <v>4</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="G57" s="1"/>
       <c r="I57" s="1"/>
@@ -4466,13 +4466,13 @@
     </row>
     <row r="58" spans="1:16" ht="158.4">
       <c r="A58" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="D58" s="24" t="s">
         <v>14</v>
@@ -4491,13 +4491,13 @@
     </row>
     <row r="59" spans="1:16" ht="158.4">
       <c r="A59" s="1" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="D59" s="24">
         <v>0</v>
@@ -4520,169 +4520,169 @@
     </row>
     <row r="60" spans="1:16" ht="72">
       <c r="A60" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="D60" s="27" t="s">
+        <v>430</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G60" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="H60" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I60" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="J60" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K60" s="32" t="s">
         <v>432</v>
       </c>
-      <c r="E60" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F60" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G60" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="H60" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="I60" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="J60" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="K60" s="32" t="s">
+      <c r="L60" s="33" t="s">
+        <v>433</v>
+      </c>
+      <c r="M60" s="1" t="s">
         <v>434</v>
-      </c>
-      <c r="L60" s="33" t="s">
-        <v>435</v>
-      </c>
-      <c r="M60" s="1" t="s">
-        <v>436</v>
       </c>
       <c r="N60" s="25"/>
       <c r="O60" s="25"/>
     </row>
     <row r="61" spans="1:16" ht="72">
       <c r="A61" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B61" s="24" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="D61" s="27" t="s">
+        <v>430</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G61" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H61" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I61" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J61" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K61" s="32" t="s">
         <v>432</v>
       </c>
-      <c r="E61" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F61" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G61" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H61" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="I61" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="J61" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="K61" s="32" t="s">
+      <c r="L61" s="33" t="s">
+        <v>433</v>
+      </c>
+      <c r="M61" s="1" t="s">
         <v>434</v>
-      </c>
-      <c r="L61" s="33" t="s">
-        <v>435</v>
-      </c>
-      <c r="M61" s="1" t="s">
-        <v>436</v>
       </c>
       <c r="N61" s="25"/>
       <c r="O61" s="25"/>
     </row>
     <row r="62" spans="1:16" ht="115.2">
       <c r="A62" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="D62" s="27" t="s">
+        <v>430</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G62" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H62" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I62" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J62" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="K62" s="32" t="s">
         <v>432</v>
       </c>
-      <c r="E62" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F62" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G62" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="H62" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="I62" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="J62" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="K62" s="32" t="s">
+      <c r="L62" s="33" t="s">
+        <v>433</v>
+      </c>
+      <c r="M62" s="1" t="s">
         <v>434</v>
-      </c>
-      <c r="L62" s="33" t="s">
-        <v>435</v>
-      </c>
-      <c r="M62" s="1" t="s">
-        <v>436</v>
       </c>
       <c r="N62" s="25"/>
       <c r="O62" s="25"/>
     </row>
     <row r="63" spans="1:16" ht="72">
       <c r="A63" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="D63" s="27" t="s">
+        <v>431</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G63" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H63" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I63" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="J63" s="32" t="s">
+        <v>432</v>
+      </c>
+      <c r="K63" s="33" t="s">
         <v>433</v>
       </c>
-      <c r="E63" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="F63" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G63" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="H63" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="I63" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="J63" s="32" t="s">
+      <c r="L63" s="1" t="s">
         <v>434</v>
-      </c>
-      <c r="K63" s="33" t="s">
-        <v>435</v>
-      </c>
-      <c r="L63" s="1" t="s">
-        <v>436</v>
       </c>
       <c r="M63" s="25"/>
       <c r="N63" s="25"/>
@@ -4690,36 +4690,36 @@
     </row>
     <row r="64" spans="1:16" ht="28.8">
       <c r="A64" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="B64" s="24" t="s">
+        <v>455</v>
+      </c>
+      <c r="C64" s="1" t="s">
         <v>456</v>
-      </c>
-      <c r="B64" s="24" t="s">
-        <v>457</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>458</v>
       </c>
       <c r="D64" s="24" t="s">
         <v>4</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="43.2">
       <c r="A65" s="1" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="B65" s="24" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="C65" s="24" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="D65" s="24" t="s">
         <v>4</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
   </sheetData>
@@ -4828,10 +4828,10 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>79</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>80</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>1</v>
@@ -4839,178 +4839,178 @@
     </row>
     <row r="2" spans="1:3" ht="43.2">
       <c r="A2" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="28.8">
       <c r="A3" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="57.6" customHeight="1">
       <c r="A4" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>84</v>
-      </c>
       <c r="C4" s="3" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="58.2" customHeight="1">
       <c r="A5" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="43.2">
       <c r="A6" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="C6" s="3" t="s">
         <v>87</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="43.2">
       <c r="A7" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>89</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="28.8">
       <c r="A8" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>91</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="57.6">
       <c r="A9" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>93</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="14.4" customHeight="1">
       <c r="A10" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B10" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>95</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="28.8">
       <c r="A11" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="28.8">
       <c r="A12" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="C12" s="3" t="s">
         <v>99</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="28.8">
       <c r="A13" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B13" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>101</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="43.2">
       <c r="A14" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B14" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>103</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="28.8">
       <c r="A15" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="28.8">
       <c r="A16" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B16" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>106</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B17" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>108</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -5040,7 +5040,7 @@
   <sheetData>
     <row r="1" spans="1:25" ht="14.25" customHeight="1">
       <c r="A1" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -5069,12 +5069,12 @@
     </row>
     <row r="2" spans="1:25" ht="14.25" customHeight="1">
       <c r="A2" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
       <c r="D2" s="10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E2" s="9"/>
       <c r="F2" s="6"/>
@@ -5100,7 +5100,7 @@
     </row>
     <row r="3" spans="1:25" ht="14.25" customHeight="1">
       <c r="A3" s="11" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B3" s="12"/>
       <c r="C3" s="12"/>
@@ -5135,13 +5135,13 @@
         <v>2</v>
       </c>
       <c r="C4" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="D4" s="17" t="s">
         <v>129</v>
       </c>
-      <c r="D4" s="17" t="s">
+      <c r="E4" s="16" t="s">
         <v>130</v>
-      </c>
-      <c r="E4" s="16" t="s">
-        <v>131</v>
       </c>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
@@ -5165,16 +5165,16 @@
       <c r="Y4" s="6"/>
     </row>
     <row r="5" spans="1:25" ht="14.25" customHeight="1">
-      <c r="A5" s="39" t="s">
+      <c r="A5" s="40" t="s">
+        <v>131</v>
+      </c>
+      <c r="B5" s="41"/>
+      <c r="C5" s="41"/>
+      <c r="D5" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="B5" s="40"/>
-      <c r="C5" s="40"/>
-      <c r="D5" s="13" t="s">
+      <c r="E5" s="13" t="s">
         <v>133</v>
-      </c>
-      <c r="E5" s="13" t="s">
-        <v>134</v>
       </c>
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
@@ -5200,14 +5200,14 @@
     <row r="6" spans="1:25" ht="14.25" customHeight="1">
       <c r="A6" s="18"/>
       <c r="B6" s="36" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C6" s="37"/>
       <c r="D6" s="38" t="s">
+        <v>135</v>
+      </c>
+      <c r="E6" s="38" t="s">
         <v>136</v>
-      </c>
-      <c r="E6" s="38" t="s">
-        <v>137</v>
       </c>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
@@ -5234,7 +5234,7 @@
       <c r="A7" s="18"/>
       <c r="B7" s="19"/>
       <c r="C7" s="19" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D7" s="37"/>
       <c r="E7" s="37"/>
@@ -5262,14 +5262,14 @@
     <row r="8" spans="1:25" ht="14.25" customHeight="1">
       <c r="A8" s="18"/>
       <c r="B8" s="36" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C8" s="37"/>
       <c r="D8" s="38" t="s">
+        <v>139</v>
+      </c>
+      <c r="E8" s="38" t="s">
         <v>140</v>
-      </c>
-      <c r="E8" s="38" t="s">
-        <v>141</v>
       </c>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
@@ -5296,7 +5296,7 @@
       <c r="A9" s="18"/>
       <c r="B9" s="19"/>
       <c r="C9" s="19" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D9" s="37"/>
       <c r="E9" s="37"/>
@@ -5324,14 +5324,14 @@
     <row r="10" spans="1:25" ht="14.25" customHeight="1">
       <c r="A10" s="18"/>
       <c r="B10" s="36" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C10" s="37"/>
       <c r="D10" s="38" t="s">
+        <v>143</v>
+      </c>
+      <c r="E10" s="38" t="s">
         <v>144</v>
-      </c>
-      <c r="E10" s="38" t="s">
-        <v>145</v>
       </c>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
@@ -5358,7 +5358,7 @@
       <c r="A11" s="18"/>
       <c r="B11" s="19"/>
       <c r="C11" s="19" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D11" s="37"/>
       <c r="E11" s="37"/>
@@ -5384,16 +5384,16 @@
       <c r="Y11" s="6"/>
     </row>
     <row r="12" spans="1:25" ht="14.25" customHeight="1">
-      <c r="A12" s="39" t="s">
+      <c r="A12" s="40" t="s">
+        <v>146</v>
+      </c>
+      <c r="B12" s="41"/>
+      <c r="C12" s="41"/>
+      <c r="D12" s="13" t="s">
         <v>147</v>
       </c>
-      <c r="B12" s="40"/>
-      <c r="C12" s="40"/>
-      <c r="D12" s="13" t="s">
+      <c r="E12" s="13" t="s">
         <v>148</v>
-      </c>
-      <c r="E12" s="13" t="s">
-        <v>149</v>
       </c>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
@@ -5419,11 +5419,11 @@
     <row r="13" spans="1:25" ht="14.25" customHeight="1">
       <c r="A13" s="18"/>
       <c r="B13" s="36" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C13" s="37"/>
       <c r="D13" s="38" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E13" s="38"/>
       <c r="F13" s="6"/>
@@ -5451,7 +5451,7 @@
       <c r="A14" s="18"/>
       <c r="B14" s="18"/>
       <c r="C14" s="19" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D14" s="37"/>
       <c r="E14" s="37"/>
@@ -5479,14 +5479,14 @@
     <row r="15" spans="1:25" ht="14.25" customHeight="1">
       <c r="A15" s="18"/>
       <c r="B15" s="36" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C15" s="37"/>
       <c r="D15" s="38" t="s">
+        <v>153</v>
+      </c>
+      <c r="E15" s="38" t="s">
         <v>154</v>
-      </c>
-      <c r="E15" s="38" t="s">
-        <v>155</v>
       </c>
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
@@ -5513,7 +5513,7 @@
       <c r="A16" s="18"/>
       <c r="B16" s="18"/>
       <c r="C16" s="19" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D16" s="37"/>
       <c r="E16" s="37"/>
@@ -5541,14 +5541,14 @@
     <row r="17" spans="1:25" ht="14.25" customHeight="1">
       <c r="A17" s="18"/>
       <c r="B17" s="36" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C17" s="37"/>
       <c r="D17" s="38" t="s">
+        <v>157</v>
+      </c>
+      <c r="E17" s="38" t="s">
         <v>158</v>
-      </c>
-      <c r="E17" s="38" t="s">
-        <v>159</v>
       </c>
       <c r="F17" s="6"/>
       <c r="G17" s="6"/>
@@ -5575,7 +5575,7 @@
       <c r="A18" s="18"/>
       <c r="B18" s="18"/>
       <c r="C18" s="19" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D18" s="37"/>
       <c r="E18" s="37"/>
@@ -5603,14 +5603,14 @@
     <row r="19" spans="1:25" ht="14.25" customHeight="1">
       <c r="A19" s="18"/>
       <c r="B19" s="36" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C19" s="37"/>
       <c r="D19" s="38" t="s">
+        <v>161</v>
+      </c>
+      <c r="E19" s="38" t="s">
         <v>162</v>
-      </c>
-      <c r="E19" s="38" t="s">
-        <v>163</v>
       </c>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
@@ -5637,7 +5637,7 @@
       <c r="A20" s="18"/>
       <c r="B20" s="18"/>
       <c r="C20" s="19" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D20" s="37"/>
       <c r="E20" s="37"/>
@@ -5663,16 +5663,16 @@
       <c r="Y20" s="6"/>
     </row>
     <row r="21" spans="1:25" ht="14.25" customHeight="1">
-      <c r="A21" s="39" t="s">
+      <c r="A21" s="40" t="s">
+        <v>164</v>
+      </c>
+      <c r="B21" s="41"/>
+      <c r="C21" s="41"/>
+      <c r="D21" s="13" t="s">
         <v>165</v>
       </c>
-      <c r="B21" s="40"/>
-      <c r="C21" s="40"/>
-      <c r="D21" s="13" t="s">
+      <c r="E21" s="13" t="s">
         <v>166</v>
-      </c>
-      <c r="E21" s="13" t="s">
-        <v>167</v>
       </c>
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
@@ -5698,14 +5698,14 @@
     <row r="22" spans="1:25" ht="14.25" customHeight="1">
       <c r="A22" s="18"/>
       <c r="B22" s="36" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C22" s="37"/>
       <c r="D22" s="38" t="s">
+        <v>168</v>
+      </c>
+      <c r="E22" s="38" t="s">
         <v>169</v>
-      </c>
-      <c r="E22" s="38" t="s">
-        <v>170</v>
       </c>
       <c r="F22" s="6"/>
       <c r="G22" s="6"/>
@@ -5732,7 +5732,7 @@
       <c r="A23" s="18"/>
       <c r="B23" s="18"/>
       <c r="C23" s="19" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D23" s="37"/>
       <c r="E23" s="37"/>
@@ -5760,14 +5760,14 @@
     <row r="24" spans="1:25" ht="14.25" customHeight="1">
       <c r="A24" s="18"/>
       <c r="B24" s="36" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C24" s="37"/>
       <c r="D24" s="38" t="s">
+        <v>172</v>
+      </c>
+      <c r="E24" s="38" t="s">
         <v>173</v>
-      </c>
-      <c r="E24" s="38" t="s">
-        <v>174</v>
       </c>
       <c r="F24" s="6"/>
       <c r="G24" s="6"/>
@@ -5794,7 +5794,7 @@
       <c r="A25" s="18"/>
       <c r="B25" s="18"/>
       <c r="C25" s="19" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D25" s="37"/>
       <c r="E25" s="37"/>
@@ -5822,14 +5822,14 @@
     <row r="26" spans="1:25" ht="14.25" customHeight="1">
       <c r="A26" s="18"/>
       <c r="B26" s="36" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C26" s="37"/>
       <c r="D26" s="38" t="s">
+        <v>176</v>
+      </c>
+      <c r="E26" s="38" t="s">
         <v>177</v>
-      </c>
-      <c r="E26" s="38" t="s">
-        <v>178</v>
       </c>
       <c r="F26" s="6"/>
       <c r="G26" s="6"/>
@@ -5856,7 +5856,7 @@
       <c r="A27" s="18"/>
       <c r="B27" s="18"/>
       <c r="C27" s="19" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D27" s="37"/>
       <c r="E27" s="37"/>
@@ -5882,16 +5882,16 @@
       <c r="Y27" s="6"/>
     </row>
     <row r="28" spans="1:25" ht="14.25" customHeight="1">
-      <c r="A28" s="39" t="s">
+      <c r="A28" s="40" t="s">
+        <v>179</v>
+      </c>
+      <c r="B28" s="41"/>
+      <c r="C28" s="41"/>
+      <c r="D28" s="13" t="s">
         <v>180</v>
       </c>
-      <c r="B28" s="40"/>
-      <c r="C28" s="40"/>
-      <c r="D28" s="13" t="s">
+      <c r="E28" s="13" t="s">
         <v>181</v>
-      </c>
-      <c r="E28" s="13" t="s">
-        <v>182</v>
       </c>
       <c r="F28" s="6"/>
       <c r="G28" s="6"/>
@@ -5917,14 +5917,14 @@
     <row r="29" spans="1:25" ht="14.25" customHeight="1">
       <c r="A29" s="18"/>
       <c r="B29" s="36" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C29" s="37"/>
       <c r="D29" s="38" t="s">
+        <v>183</v>
+      </c>
+      <c r="E29" s="38" t="s">
         <v>184</v>
-      </c>
-      <c r="E29" s="38" t="s">
-        <v>185</v>
       </c>
       <c r="F29" s="6"/>
       <c r="G29" s="6"/>
@@ -5951,7 +5951,7 @@
       <c r="A30" s="18"/>
       <c r="B30" s="18"/>
       <c r="C30" s="19" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D30" s="37"/>
       <c r="E30" s="37"/>
@@ -5979,14 +5979,14 @@
     <row r="31" spans="1:25" ht="14.25" customHeight="1">
       <c r="A31" s="18"/>
       <c r="B31" s="36" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C31" s="37"/>
       <c r="D31" s="38" t="s">
+        <v>187</v>
+      </c>
+      <c r="E31" s="38" t="s">
         <v>188</v>
-      </c>
-      <c r="E31" s="38" t="s">
-        <v>189</v>
       </c>
       <c r="F31" s="6"/>
       <c r="G31" s="6"/>
@@ -6013,7 +6013,7 @@
       <c r="A32" s="18"/>
       <c r="B32" s="18"/>
       <c r="C32" s="19" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D32" s="37"/>
       <c r="E32" s="37"/>
@@ -6041,14 +6041,14 @@
     <row r="33" spans="1:25" ht="14.25" customHeight="1">
       <c r="A33" s="18"/>
       <c r="B33" s="36" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C33" s="37"/>
       <c r="D33" s="38" t="s">
+        <v>191</v>
+      </c>
+      <c r="E33" s="38" t="s">
         <v>192</v>
-      </c>
-      <c r="E33" s="38" t="s">
-        <v>193</v>
       </c>
       <c r="F33" s="6"/>
       <c r="G33" s="6"/>
@@ -6075,7 +6075,7 @@
       <c r="A34" s="18"/>
       <c r="B34" s="18"/>
       <c r="C34" s="19" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D34" s="37"/>
       <c r="E34" s="37"/>
@@ -6103,14 +6103,14 @@
     <row r="35" spans="1:25" ht="14.25" customHeight="1">
       <c r="A35" s="18"/>
       <c r="B35" s="36" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C35" s="37"/>
       <c r="D35" s="38" t="s">
+        <v>195</v>
+      </c>
+      <c r="E35" s="38" t="s">
         <v>196</v>
-      </c>
-      <c r="E35" s="38" t="s">
-        <v>197</v>
       </c>
       <c r="F35" s="6"/>
       <c r="G35" s="6"/>
@@ -6137,7 +6137,7 @@
       <c r="A36" s="18"/>
       <c r="B36" s="18"/>
       <c r="C36" s="19" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D36" s="37"/>
       <c r="E36" s="37"/>
@@ -6163,16 +6163,16 @@
       <c r="Y36" s="6"/>
     </row>
     <row r="37" spans="1:25" ht="14.25" customHeight="1">
-      <c r="A37" s="39" t="s">
+      <c r="A37" s="40" t="s">
+        <v>198</v>
+      </c>
+      <c r="B37" s="41"/>
+      <c r="C37" s="41"/>
+      <c r="D37" s="13" t="s">
         <v>199</v>
       </c>
-      <c r="B37" s="40"/>
-      <c r="C37" s="40"/>
-      <c r="D37" s="13" t="s">
+      <c r="E37" s="13" t="s">
         <v>200</v>
-      </c>
-      <c r="E37" s="13" t="s">
-        <v>201</v>
       </c>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
@@ -6198,14 +6198,14 @@
     <row r="38" spans="1:25" ht="14.25" customHeight="1">
       <c r="A38" s="18"/>
       <c r="B38" s="36" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C38" s="37"/>
       <c r="D38" s="38" t="s">
+        <v>202</v>
+      </c>
+      <c r="E38" s="38" t="s">
         <v>203</v>
-      </c>
-      <c r="E38" s="38" t="s">
-        <v>204</v>
       </c>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
@@ -6232,7 +6232,7 @@
       <c r="A39" s="18"/>
       <c r="B39" s="18"/>
       <c r="C39" s="19" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D39" s="37"/>
       <c r="E39" s="37"/>
@@ -6260,14 +6260,14 @@
     <row r="40" spans="1:25" ht="14.25" customHeight="1">
       <c r="A40" s="18"/>
       <c r="B40" s="36" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C40" s="37"/>
       <c r="D40" s="38" t="s">
+        <v>206</v>
+      </c>
+      <c r="E40" s="38" t="s">
         <v>207</v>
-      </c>
-      <c r="E40" s="38" t="s">
-        <v>208</v>
       </c>
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
@@ -6294,7 +6294,7 @@
       <c r="A41" s="18"/>
       <c r="B41" s="18"/>
       <c r="C41" s="19" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D41" s="37"/>
       <c r="E41" s="37"/>
@@ -6322,14 +6322,14 @@
     <row r="42" spans="1:25" ht="14.25" customHeight="1">
       <c r="A42" s="18"/>
       <c r="B42" s="36" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C42" s="37"/>
       <c r="D42" s="38" t="s">
+        <v>210</v>
+      </c>
+      <c r="E42" s="38" t="s">
         <v>211</v>
-      </c>
-      <c r="E42" s="38" t="s">
-        <v>212</v>
       </c>
       <c r="F42" s="6"/>
       <c r="G42" s="6"/>
@@ -6356,7 +6356,7 @@
       <c r="A43" s="18"/>
       <c r="B43" s="18"/>
       <c r="C43" s="19" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D43" s="37"/>
       <c r="E43" s="37"/>
@@ -6384,14 +6384,14 @@
     <row r="44" spans="1:25" ht="14.25" customHeight="1">
       <c r="A44" s="18"/>
       <c r="B44" s="36" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C44" s="37"/>
       <c r="D44" s="38" t="s">
+        <v>214</v>
+      </c>
+      <c r="E44" s="38" t="s">
         <v>215</v>
-      </c>
-      <c r="E44" s="38" t="s">
-        <v>216</v>
       </c>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
@@ -6418,7 +6418,7 @@
       <c r="A45" s="18"/>
       <c r="B45" s="18"/>
       <c r="C45" s="19" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D45" s="37"/>
       <c r="E45" s="37"/>
@@ -6444,16 +6444,16 @@
       <c r="Y45" s="6"/>
     </row>
     <row r="46" spans="1:25" ht="14.25" customHeight="1">
-      <c r="A46" s="39" t="s">
+      <c r="A46" s="40" t="s">
+        <v>217</v>
+      </c>
+      <c r="B46" s="41"/>
+      <c r="C46" s="41"/>
+      <c r="D46" s="13" t="s">
         <v>218</v>
       </c>
-      <c r="B46" s="40"/>
-      <c r="C46" s="40"/>
-      <c r="D46" s="13" t="s">
+      <c r="E46" s="13" t="s">
         <v>219</v>
-      </c>
-      <c r="E46" s="13" t="s">
-        <v>220</v>
       </c>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
@@ -6479,14 +6479,14 @@
     <row r="47" spans="1:25" ht="14.25" customHeight="1">
       <c r="A47" s="18"/>
       <c r="B47" s="36" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C47" s="37"/>
       <c r="D47" s="38" t="s">
+        <v>221</v>
+      </c>
+      <c r="E47" s="38" t="s">
         <v>222</v>
-      </c>
-      <c r="E47" s="38" t="s">
-        <v>223</v>
       </c>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
@@ -6513,7 +6513,7 @@
       <c r="A48" s="18"/>
       <c r="B48" s="18"/>
       <c r="C48" s="19" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D48" s="37"/>
       <c r="E48" s="37"/>
@@ -6541,14 +6541,14 @@
     <row r="49" spans="1:25" ht="14.25" customHeight="1">
       <c r="A49" s="18"/>
       <c r="B49" s="36" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C49" s="37"/>
       <c r="D49" s="38" t="s">
+        <v>225</v>
+      </c>
+      <c r="E49" s="38" t="s">
         <v>226</v>
-      </c>
-      <c r="E49" s="38" t="s">
-        <v>227</v>
       </c>
       <c r="F49" s="6"/>
       <c r="G49" s="6"/>
@@ -6575,7 +6575,7 @@
       <c r="A50" s="18"/>
       <c r="B50" s="18"/>
       <c r="C50" s="19" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D50" s="37"/>
       <c r="E50" s="37"/>
@@ -6603,14 +6603,14 @@
     <row r="51" spans="1:25" ht="14.25" customHeight="1">
       <c r="A51" s="18"/>
       <c r="B51" s="36" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C51" s="37"/>
       <c r="D51" s="38" t="s">
+        <v>229</v>
+      </c>
+      <c r="E51" s="38" t="s">
         <v>230</v>
-      </c>
-      <c r="E51" s="38" t="s">
-        <v>231</v>
       </c>
       <c r="F51" s="6"/>
       <c r="G51" s="6"/>
@@ -6637,7 +6637,7 @@
       <c r="A52" s="18"/>
       <c r="B52" s="18"/>
       <c r="C52" s="19" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D52" s="37"/>
       <c r="E52" s="37"/>
@@ -6663,16 +6663,16 @@
       <c r="Y52" s="6"/>
     </row>
     <row r="53" spans="1:25" ht="14.25" customHeight="1">
-      <c r="A53" s="39" t="s">
+      <c r="A53" s="40" t="s">
+        <v>232</v>
+      </c>
+      <c r="B53" s="41"/>
+      <c r="C53" s="41"/>
+      <c r="D53" s="13" t="s">
         <v>233</v>
       </c>
-      <c r="B53" s="40"/>
-      <c r="C53" s="40"/>
-      <c r="D53" s="13" t="s">
+      <c r="E53" s="13" t="s">
         <v>234</v>
-      </c>
-      <c r="E53" s="13" t="s">
-        <v>235</v>
       </c>
       <c r="F53" s="6"/>
       <c r="G53" s="6"/>
@@ -6698,14 +6698,14 @@
     <row r="54" spans="1:25" ht="14.25" customHeight="1">
       <c r="A54" s="18"/>
       <c r="B54" s="36" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C54" s="37"/>
       <c r="D54" s="38" t="s">
+        <v>236</v>
+      </c>
+      <c r="E54" s="38" t="s">
         <v>237</v>
-      </c>
-      <c r="E54" s="38" t="s">
-        <v>238</v>
       </c>
       <c r="F54" s="6"/>
       <c r="G54" s="6"/>
@@ -6732,7 +6732,7 @@
       <c r="A55" s="18"/>
       <c r="B55" s="18"/>
       <c r="C55" s="19" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D55" s="37"/>
       <c r="E55" s="37"/>
@@ -6760,14 +6760,14 @@
     <row r="56" spans="1:25" ht="14.25" customHeight="1">
       <c r="A56" s="18"/>
       <c r="B56" s="36" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C56" s="37"/>
       <c r="D56" s="38" t="s">
+        <v>240</v>
+      </c>
+      <c r="E56" s="38" t="s">
         <v>241</v>
-      </c>
-      <c r="E56" s="38" t="s">
-        <v>242</v>
       </c>
       <c r="F56" s="6"/>
       <c r="G56" s="6"/>
@@ -6794,7 +6794,7 @@
       <c r="A57" s="18"/>
       <c r="B57" s="18"/>
       <c r="C57" s="19" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D57" s="37"/>
       <c r="E57" s="37"/>
@@ -6822,11 +6822,11 @@
     <row r="58" spans="1:25" ht="14.25" customHeight="1">
       <c r="A58" s="18"/>
       <c r="B58" s="36" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C58" s="37"/>
       <c r="D58" s="38" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E58" s="38"/>
       <c r="F58" s="6"/>
@@ -6854,7 +6854,7 @@
       <c r="A59" s="18"/>
       <c r="B59" s="18"/>
       <c r="C59" s="19" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D59" s="37"/>
       <c r="E59" s="37"/>
@@ -6880,16 +6880,16 @@
       <c r="Y59" s="6"/>
     </row>
     <row r="60" spans="1:25" ht="14.25" customHeight="1">
-      <c r="A60" s="39" t="s">
+      <c r="A60" s="40" t="s">
+        <v>246</v>
+      </c>
+      <c r="B60" s="41"/>
+      <c r="C60" s="41"/>
+      <c r="D60" s="13" t="s">
         <v>247</v>
       </c>
-      <c r="B60" s="40"/>
-      <c r="C60" s="40"/>
-      <c r="D60" s="13" t="s">
+      <c r="E60" s="13" t="s">
         <v>248</v>
-      </c>
-      <c r="E60" s="13" t="s">
-        <v>249</v>
       </c>
       <c r="F60" s="6"/>
       <c r="G60" s="6"/>
@@ -6915,14 +6915,14 @@
     <row r="61" spans="1:25" ht="14.25" customHeight="1">
       <c r="A61" s="18"/>
       <c r="B61" s="36" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C61" s="37"/>
       <c r="D61" s="38" t="s">
+        <v>250</v>
+      </c>
+      <c r="E61" s="38" t="s">
         <v>251</v>
-      </c>
-      <c r="E61" s="38" t="s">
-        <v>252</v>
       </c>
       <c r="F61" s="6"/>
       <c r="G61" s="6"/>
@@ -6949,7 +6949,7 @@
       <c r="A62" s="18"/>
       <c r="B62" s="18"/>
       <c r="C62" s="19" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D62" s="37"/>
       <c r="E62" s="37"/>
@@ -6977,14 +6977,14 @@
     <row r="63" spans="1:25" ht="14.25" customHeight="1">
       <c r="A63" s="18"/>
       <c r="B63" s="36" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C63" s="37"/>
       <c r="D63" s="38" t="s">
+        <v>254</v>
+      </c>
+      <c r="E63" s="38" t="s">
         <v>255</v>
-      </c>
-      <c r="E63" s="38" t="s">
-        <v>256</v>
       </c>
       <c r="F63" s="6"/>
       <c r="G63" s="6"/>
@@ -7011,7 +7011,7 @@
       <c r="A64" s="18"/>
       <c r="B64" s="18"/>
       <c r="C64" s="19" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D64" s="37"/>
       <c r="E64" s="37"/>
@@ -7039,14 +7039,14 @@
     <row r="65" spans="1:25" ht="14.25" customHeight="1">
       <c r="A65" s="18"/>
       <c r="B65" s="36" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C65" s="37"/>
       <c r="D65" s="38" t="s">
+        <v>258</v>
+      </c>
+      <c r="E65" s="38" t="s">
         <v>259</v>
-      </c>
-      <c r="E65" s="38" t="s">
-        <v>260</v>
       </c>
       <c r="F65" s="6"/>
       <c r="G65" s="6"/>
@@ -7073,7 +7073,7 @@
       <c r="A66" s="18"/>
       <c r="B66" s="18"/>
       <c r="C66" s="19" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D66" s="37"/>
       <c r="E66" s="37"/>
@@ -7099,16 +7099,16 @@
       <c r="Y66" s="6"/>
     </row>
     <row r="67" spans="1:25" ht="14.25" customHeight="1">
-      <c r="A67" s="39" t="s">
+      <c r="A67" s="40" t="s">
+        <v>261</v>
+      </c>
+      <c r="B67" s="41"/>
+      <c r="C67" s="41"/>
+      <c r="D67" s="13" t="s">
         <v>262</v>
       </c>
-      <c r="B67" s="40"/>
-      <c r="C67" s="40"/>
-      <c r="D67" s="13" t="s">
+      <c r="E67" s="13" t="s">
         <v>263</v>
-      </c>
-      <c r="E67" s="13" t="s">
-        <v>264</v>
       </c>
       <c r="F67" s="6"/>
       <c r="G67" s="6"/>
@@ -7134,14 +7134,14 @@
     <row r="68" spans="1:25" ht="14.25" customHeight="1">
       <c r="A68" s="18"/>
       <c r="B68" s="36" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C68" s="37"/>
       <c r="D68" s="38" t="s">
+        <v>265</v>
+      </c>
+      <c r="E68" s="38" t="s">
         <v>266</v>
-      </c>
-      <c r="E68" s="38" t="s">
-        <v>267</v>
       </c>
       <c r="F68" s="6"/>
       <c r="G68" s="6"/>
@@ -7168,7 +7168,7 @@
       <c r="A69" s="18"/>
       <c r="B69" s="18"/>
       <c r="C69" s="19" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D69" s="37"/>
       <c r="E69" s="37"/>
@@ -7196,14 +7196,14 @@
     <row r="70" spans="1:25" ht="14.25" customHeight="1">
       <c r="A70" s="18"/>
       <c r="B70" s="36" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C70" s="37"/>
       <c r="D70" s="38" t="s">
+        <v>269</v>
+      </c>
+      <c r="E70" s="38" t="s">
         <v>270</v>
-      </c>
-      <c r="E70" s="38" t="s">
-        <v>271</v>
       </c>
       <c r="F70" s="6"/>
       <c r="G70" s="6"/>
@@ -7230,7 +7230,7 @@
       <c r="A71" s="18"/>
       <c r="B71" s="18"/>
       <c r="C71" s="19" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D71" s="37"/>
       <c r="E71" s="37"/>
@@ -7258,14 +7258,14 @@
     <row r="72" spans="1:25" ht="14.25" customHeight="1">
       <c r="A72" s="18"/>
       <c r="B72" s="36" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C72" s="37"/>
       <c r="D72" s="38" t="s">
+        <v>273</v>
+      </c>
+      <c r="E72" s="38" t="s">
         <v>274</v>
-      </c>
-      <c r="E72" s="38" t="s">
-        <v>275</v>
       </c>
       <c r="F72" s="6"/>
       <c r="G72" s="6"/>
@@ -7292,7 +7292,7 @@
       <c r="A73" s="18"/>
       <c r="B73" s="18"/>
       <c r="C73" s="19" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D73" s="37"/>
       <c r="E73" s="37"/>
@@ -7320,14 +7320,14 @@
     <row r="74" spans="1:25" ht="14.25" customHeight="1">
       <c r="A74" s="18"/>
       <c r="B74" s="36" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C74" s="37"/>
       <c r="D74" s="38" t="s">
+        <v>277</v>
+      </c>
+      <c r="E74" s="38" t="s">
         <v>278</v>
-      </c>
-      <c r="E74" s="38" t="s">
-        <v>279</v>
       </c>
       <c r="F74" s="6"/>
       <c r="G74" s="6"/>
@@ -7354,7 +7354,7 @@
       <c r="A75" s="18"/>
       <c r="B75" s="18"/>
       <c r="C75" s="19" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D75" s="37"/>
       <c r="E75" s="37"/>
@@ -7382,14 +7382,14 @@
     <row r="76" spans="1:25" ht="14.25" customHeight="1">
       <c r="A76" s="18"/>
       <c r="B76" s="36" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C76" s="37"/>
       <c r="D76" s="38" t="s">
+        <v>281</v>
+      </c>
+      <c r="E76" s="38" t="s">
         <v>282</v>
-      </c>
-      <c r="E76" s="38" t="s">
-        <v>283</v>
       </c>
       <c r="F76" s="6"/>
       <c r="G76" s="6"/>
@@ -7416,7 +7416,7 @@
       <c r="A77" s="18"/>
       <c r="B77" s="18"/>
       <c r="C77" s="19" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D77" s="37"/>
       <c r="E77" s="37"/>
@@ -7444,14 +7444,14 @@
     <row r="78" spans="1:25" ht="14.25" customHeight="1">
       <c r="A78" s="18"/>
       <c r="B78" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C78" s="37"/>
       <c r="D78" s="38" t="s">
+        <v>285</v>
+      </c>
+      <c r="E78" s="38" t="s">
         <v>286</v>
-      </c>
-      <c r="E78" s="38" t="s">
-        <v>287</v>
       </c>
       <c r="F78" s="6"/>
       <c r="G78" s="6"/>
@@ -7478,7 +7478,7 @@
       <c r="A79" s="18"/>
       <c r="B79" s="18"/>
       <c r="C79" s="19" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D79" s="37"/>
       <c r="E79" s="37"/>
@@ -7504,16 +7504,16 @@
       <c r="Y79" s="6"/>
     </row>
     <row r="80" spans="1:25" ht="14.25" customHeight="1">
-      <c r="A80" s="39" t="s">
+      <c r="A80" s="40" t="s">
+        <v>288</v>
+      </c>
+      <c r="B80" s="41"/>
+      <c r="C80" s="41"/>
+      <c r="D80" s="13" t="s">
         <v>289</v>
       </c>
-      <c r="B80" s="40"/>
-      <c r="C80" s="40"/>
-      <c r="D80" s="13" t="s">
+      <c r="E80" s="13" t="s">
         <v>290</v>
-      </c>
-      <c r="E80" s="13" t="s">
-        <v>291</v>
       </c>
       <c r="F80" s="6"/>
       <c r="G80" s="6"/>
@@ -7539,11 +7539,11 @@
     <row r="81" spans="1:25" ht="14.25" customHeight="1">
       <c r="A81" s="18"/>
       <c r="B81" s="36" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C81" s="37"/>
       <c r="D81" s="38" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E81" s="38"/>
       <c r="F81" s="6"/>
@@ -7571,7 +7571,7 @@
       <c r="A82" s="18"/>
       <c r="B82" s="18"/>
       <c r="C82" s="19" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D82" s="37"/>
       <c r="E82" s="37"/>
@@ -7599,11 +7599,11 @@
     <row r="83" spans="1:25" ht="14.25" customHeight="1">
       <c r="A83" s="18"/>
       <c r="B83" s="36" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C83" s="37"/>
       <c r="D83" s="38" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E83" s="38"/>
       <c r="F83" s="6"/>
@@ -7631,7 +7631,7 @@
       <c r="A84" s="18"/>
       <c r="B84" s="18"/>
       <c r="C84" s="19" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D84" s="37"/>
       <c r="E84" s="37"/>
@@ -7659,11 +7659,11 @@
     <row r="85" spans="1:25" ht="14.25" customHeight="1">
       <c r="A85" s="18"/>
       <c r="B85" s="36" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C85" s="37"/>
       <c r="D85" s="38" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E85" s="38"/>
       <c r="F85" s="6"/>
@@ -7691,7 +7691,7 @@
       <c r="A86" s="18"/>
       <c r="B86" s="18"/>
       <c r="C86" s="19" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D86" s="37"/>
       <c r="E86" s="37"/>
@@ -7717,16 +7717,16 @@
       <c r="Y86" s="6"/>
     </row>
     <row r="87" spans="1:25" ht="14.25" customHeight="1">
-      <c r="A87" s="39" t="s">
+      <c r="A87" s="40" t="s">
+        <v>300</v>
+      </c>
+      <c r="B87" s="41"/>
+      <c r="C87" s="41"/>
+      <c r="D87" s="13" t="s">
         <v>301</v>
       </c>
-      <c r="B87" s="40"/>
-      <c r="C87" s="40"/>
-      <c r="D87" s="13" t="s">
+      <c r="E87" s="13" t="s">
         <v>302</v>
-      </c>
-      <c r="E87" s="13" t="s">
-        <v>303</v>
       </c>
       <c r="F87" s="6"/>
       <c r="G87" s="6"/>
@@ -7752,14 +7752,14 @@
     <row r="88" spans="1:25" ht="14.25" customHeight="1">
       <c r="A88" s="18"/>
       <c r="B88" s="36" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C88" s="37"/>
       <c r="D88" s="38" t="s">
+        <v>304</v>
+      </c>
+      <c r="E88" s="38" t="s">
         <v>305</v>
-      </c>
-      <c r="E88" s="38" t="s">
-        <v>306</v>
       </c>
       <c r="F88" s="6"/>
       <c r="G88" s="6"/>
@@ -7786,7 +7786,7 @@
       <c r="A89" s="18"/>
       <c r="B89" s="18"/>
       <c r="C89" s="19" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D89" s="37"/>
       <c r="E89" s="37"/>
@@ -7814,11 +7814,11 @@
     <row r="90" spans="1:25" ht="14.25" customHeight="1">
       <c r="A90" s="18"/>
       <c r="B90" s="36" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C90" s="37"/>
       <c r="D90" s="38" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E90" s="38"/>
       <c r="F90" s="6"/>
@@ -7846,7 +7846,7 @@
       <c r="A91" s="18"/>
       <c r="B91" s="18"/>
       <c r="C91" s="19" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D91" s="37"/>
       <c r="E91" s="37"/>
@@ -7874,11 +7874,11 @@
     <row r="92" spans="1:25" ht="14.25" customHeight="1">
       <c r="A92" s="18"/>
       <c r="B92" s="36" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C92" s="37"/>
       <c r="D92" s="38" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E92" s="38"/>
       <c r="F92" s="6"/>
@@ -7906,7 +7906,7 @@
       <c r="A93" s="18"/>
       <c r="B93" s="18"/>
       <c r="C93" s="19" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D93" s="37"/>
       <c r="E93" s="37"/>
@@ -7934,11 +7934,11 @@
     <row r="94" spans="1:25" ht="14.25" customHeight="1">
       <c r="A94" s="18"/>
       <c r="B94" s="36" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C94" s="37"/>
       <c r="D94" s="38" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="E94" s="38"/>
       <c r="F94" s="6"/>
@@ -7966,10 +7966,10 @@
       <c r="A95" s="20"/>
       <c r="B95" s="20"/>
       <c r="C95" s="21" t="s">
-        <v>316</v>
-      </c>
-      <c r="D95" s="41"/>
-      <c r="E95" s="41"/>
+        <v>315</v>
+      </c>
+      <c r="D95" s="39"/>
+      <c r="E95" s="39"/>
       <c r="F95" s="6"/>
       <c r="G95" s="6"/>
       <c r="H95" s="6"/>
@@ -14098,44 +14098,85 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="131">
-    <mergeCell ref="B92:C92"/>
-    <mergeCell ref="D92:D93"/>
-    <mergeCell ref="E92:E93"/>
-    <mergeCell ref="B94:C94"/>
-    <mergeCell ref="D94:D95"/>
-    <mergeCell ref="E94:E95"/>
-    <mergeCell ref="A87:C87"/>
-    <mergeCell ref="B88:C88"/>
-    <mergeCell ref="D88:D89"/>
-    <mergeCell ref="E88:E89"/>
-    <mergeCell ref="B90:C90"/>
-    <mergeCell ref="D90:D91"/>
-    <mergeCell ref="E90:E91"/>
-    <mergeCell ref="B83:C83"/>
-    <mergeCell ref="D83:D84"/>
-    <mergeCell ref="E83:E84"/>
-    <mergeCell ref="B85:C85"/>
-    <mergeCell ref="D85:D86"/>
-    <mergeCell ref="E85:E86"/>
-    <mergeCell ref="B78:C78"/>
-    <mergeCell ref="D78:D79"/>
-    <mergeCell ref="E78:E79"/>
-    <mergeCell ref="A80:C80"/>
-    <mergeCell ref="B81:C81"/>
-    <mergeCell ref="D81:D82"/>
-    <mergeCell ref="E81:E82"/>
-    <mergeCell ref="B74:C74"/>
-    <mergeCell ref="D74:D75"/>
-    <mergeCell ref="E74:E75"/>
-    <mergeCell ref="B76:C76"/>
-    <mergeCell ref="D76:D77"/>
-    <mergeCell ref="E76:E77"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="D70:D71"/>
-    <mergeCell ref="E70:E71"/>
-    <mergeCell ref="B72:C72"/>
-    <mergeCell ref="D72:D73"/>
-    <mergeCell ref="E72:E73"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="A37:C37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="E38:E39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="D40:D41"/>
+    <mergeCell ref="E40:E41"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="E33:E34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="E35:E36"/>
+    <mergeCell ref="A46:C46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="D47:D48"/>
+    <mergeCell ref="E47:E48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="D49:D50"/>
+    <mergeCell ref="E49:E50"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="E42:E43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="E44:E45"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="D56:D57"/>
+    <mergeCell ref="E56:E57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="D58:D59"/>
+    <mergeCell ref="E58:E59"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="D51:D52"/>
+    <mergeCell ref="E51:E52"/>
+    <mergeCell ref="A53:C53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="D54:D55"/>
+    <mergeCell ref="E54:E55"/>
     <mergeCell ref="B65:C65"/>
     <mergeCell ref="D65:D66"/>
     <mergeCell ref="E65:E66"/>
@@ -14150,85 +14191,44 @@
     <mergeCell ref="B63:C63"/>
     <mergeCell ref="D63:D64"/>
     <mergeCell ref="E63:E64"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="D56:D57"/>
-    <mergeCell ref="E56:E57"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="D58:D59"/>
-    <mergeCell ref="E58:E59"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="D51:D52"/>
-    <mergeCell ref="E51:E52"/>
-    <mergeCell ref="A53:C53"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="D54:D55"/>
-    <mergeCell ref="E54:E55"/>
-    <mergeCell ref="A46:C46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="D47:D48"/>
-    <mergeCell ref="E47:E48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="D49:D50"/>
-    <mergeCell ref="E49:E50"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="D42:D43"/>
-    <mergeCell ref="E42:E43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="D44:D45"/>
-    <mergeCell ref="E44:E45"/>
-    <mergeCell ref="A37:C37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="E38:E39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="D40:D41"/>
-    <mergeCell ref="E40:E41"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="E33:E34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="E35:E36"/>
-    <mergeCell ref="A28:C28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="E31:E32"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="B74:C74"/>
+    <mergeCell ref="D74:D75"/>
+    <mergeCell ref="E74:E75"/>
+    <mergeCell ref="B76:C76"/>
+    <mergeCell ref="D76:D77"/>
+    <mergeCell ref="E76:E77"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="D70:D71"/>
+    <mergeCell ref="E70:E71"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="D72:D73"/>
+    <mergeCell ref="E72:E73"/>
+    <mergeCell ref="B83:C83"/>
+    <mergeCell ref="D83:D84"/>
+    <mergeCell ref="E83:E84"/>
+    <mergeCell ref="B85:C85"/>
+    <mergeCell ref="D85:D86"/>
+    <mergeCell ref="E85:E86"/>
+    <mergeCell ref="B78:C78"/>
+    <mergeCell ref="D78:D79"/>
+    <mergeCell ref="E78:E79"/>
+    <mergeCell ref="A80:C80"/>
+    <mergeCell ref="B81:C81"/>
+    <mergeCell ref="D81:D82"/>
+    <mergeCell ref="E81:E82"/>
+    <mergeCell ref="B92:C92"/>
+    <mergeCell ref="D92:D93"/>
+    <mergeCell ref="E92:E93"/>
+    <mergeCell ref="B94:C94"/>
+    <mergeCell ref="D94:D95"/>
+    <mergeCell ref="E94:E95"/>
+    <mergeCell ref="A87:C87"/>
+    <mergeCell ref="B88:C88"/>
+    <mergeCell ref="D88:D89"/>
+    <mergeCell ref="E88:E89"/>
+    <mergeCell ref="B90:C90"/>
+    <mergeCell ref="D90:D91"/>
+    <mergeCell ref="E90:E91"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1"/>

</xml_diff>